<commit_message>
feat(autovalidation): add autovalidation logic for asr
</commit_message>
<xml_diff>
--- a/utils/localization/resources/backup/nextjs_meta.xlsx
+++ b/utils/localization/resources/backup/nextjs_meta.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:N384"/>
+  <dimension ref="A2:N393"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,7 +518,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>होम</t>
+          <t>होम पेज</t>
         </is>
       </c>
       <c r="D3" t="inlineStr"/>
@@ -554,7 +554,7 @@
       </c>
       <c r="K3" t="inlineStr">
         <is>
-          <t>ਮੁੱਖ ਪੰਨਾ</t>
+          <t>ਹੋਮ</t>
         </is>
       </c>
       <c r="L3" t="inlineStr">
@@ -627,7 +627,7 @@
       </c>
       <c r="L4" t="inlineStr">
         <is>
-          <t>സുനോ</t>
+          <t>കേള്‍ക്കൂ</t>
         </is>
       </c>
       <c r="M4" t="inlineStr">
@@ -695,7 +695,7 @@
       </c>
       <c r="L5" t="inlineStr">
         <is>
-          <t>ബോലോ</t>
+          <t>പറയൂ</t>
         </is>
       </c>
       <c r="M5" t="inlineStr">
@@ -763,7 +763,7 @@
       </c>
       <c r="L6" t="inlineStr">
         <is>
-          <t>ലിഖോ</t>
+          <t>എഴുതൂ</t>
         </is>
       </c>
       <c r="M6" t="inlineStr">
@@ -831,7 +831,7 @@
       </c>
       <c r="L7" t="inlineStr">
         <is>
-          <t>ദേഖോ</t>
+          <t>കാണുക</t>
         </is>
       </c>
       <c r="M7" t="inlineStr">
@@ -1350,7 +1350,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>একটি প্ল্যাটফর্ম, একাধিক ক্রাউডসোর্সিং  উদ্যোগ</t>
+          <t>একটি প্ল্যাটফর্ম, একাধিক ক্রাউডসোর্সিং উদ্যোগ</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
@@ -1481,7 +1481,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>পাঠৰ পৰা অডিঅ'লৈ প্ৰতিলিপিবদ্ধ কৰি আপোনাৰ ভাষা সমৃদ্ধ কৰক</t>
+          <t>আপুনি শুনা অডিঅ’ টাইপ কৰি আপোনাৰ ভাষাক সমৃদ্ধ কৰক</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1627,7 +1627,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>மற்றவர்களால் எழுத்துவடிவமாக்கப்பட்ட உரைகளை மதிப்பாய்வு செய்யவும்</t>
+          <t>மற்றவர்களால் டிரான்ஸ்க்ரைப் செய்யப்பட்ட உரைகளை சரிபார்க்கவும்</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1758,7 +1758,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>আপনার কন্ঠস্বর দান করে বাক্যটি রেকর্ড  করুন</t>
+          <t>আপনার কন্ঠস্বর দান করে বাক্যটি রেকর্ড করুন</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
@@ -1846,7 +1846,7 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>ਹੋਰਾਂ ਦੁਆਰਾ ਰਿਕਾਰਡ ਕੀਤੇ ਆਡੀਓ ਨੂੰ ਪ੍ਰਮਾਣਿਤ ਕਰੋ</t>
+          <t>ਰਿਕਾਰਡ ਕੀਤੇ ਗਏ ਆਡੀਓ ਨੂੰ ਪ੍ਰਮਾਣਿਤ ਕਰੋ</t>
         </is>
       </c>
       <c r="L22" t="inlineStr">
@@ -1894,7 +1894,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>লিখিত বাক্য গুলিকে অনুবাদ করে আপনার ভাষাকে সমৃদ্ধ করুন।</t>
+          <t>লিখিত বাক্য গুলিকে অনুবাদ করে আপনার ভাষাকে সমৃদ্ধ করুন</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
@@ -2050,7 +2050,7 @@
       </c>
       <c r="K25" t="inlineStr">
         <is>
-          <t>ਹੋਰਾਂ ਦੇ  ਯੋਗਦਾਨਾਂ ਵਾਲੇ ਅਨੁਵਾਦਾਂ ਨੂੰ ਪ੍ਰਮਾਣਿਤ ਕਰੋ</t>
+          <t>ਅਨੁਵਾਦਾਂ ਨੂੰ ਪ੍ਰਮਾਣਿਤ ਕਰੋ</t>
         </is>
       </c>
       <c r="L25" t="inlineStr">
@@ -2093,7 +2093,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>ছৱিসমূহত লেবেল লগাই আপোনাৰ নিজৰ ভাষা সমৃদ্ধ কৰক</t>
+          <t>আপুনি দেখা পোৱা পাঠ সমূহ টাইপ কৰি আপোনাৰ ভাষাক সমৃদ্ধ কৰক</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -2254,7 +2254,7 @@
       </c>
       <c r="K28" t="inlineStr">
         <is>
-          <t>ਹੋਰਾਂ ਦੁਆਰਾ ਲੇਬਲ ਕੀਤੀ ਗਈ ਇਮੇਜ ਨੂੰ ਪ੍ਰਮਾਣਿਤ ਕਰੋ</t>
+          <t>ਲੇਬਲ ਕੀਤੀ ਗਈ ਇਮੇਜ ਨੂੰ ਪ੍ਰਮਾਣਿਤ ਕਰੋ</t>
         </is>
       </c>
       <c r="L28" t="inlineStr">
@@ -2322,7 +2322,7 @@
       </c>
       <c r="K29" t="inlineStr">
         <is>
-          <t>ਯੋਗਦਾਨ ਦੇਣਾ ਸ਼ੁਰੂ ਕਰੋ</t>
+          <t>ਹਿੱਸਾ ਲਵੋ</t>
         </is>
       </c>
       <c r="L29" t="inlineStr">
@@ -2365,7 +2365,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Total Participation</t>
+          <t>মুঠ অংশগ্ৰহণ</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -2390,7 +2390,7 @@
       </c>
       <c r="K30" t="inlineStr">
         <is>
-          <t>ਭਾਗੀਦਾਰਾਂ ਦੀ ਕੁੱਲ ਸੰਖਿਆ</t>
+          <t>ਕੁੱਲ ਭਾਗੀਦਾਰ</t>
         </is>
       </c>
       <c r="L30" t="inlineStr">
@@ -2526,7 +2526,7 @@
       </c>
       <c r="K32" t="inlineStr">
         <is>
-          <t>ਯੋਗਦਾਨ ਪਾਓ ਅਤੇ ਭਾਸ਼ਾ ਸਮਰਥਕ ਬਣੋ</t>
+          <t>ਯੋਗਦਾਨ ਦਿਉ ਅਤੇ ਭਾਸ਼ਾ ਸਮਰਥਕ ਬਣੋ</t>
         </is>
       </c>
       <c r="L32" t="inlineStr">
@@ -2798,7 +2798,7 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>ਤੁਹਾਡਾ ਸੁਝਾਅ</t>
+          <t>ਤੁਹਾਡਾ ਫੀਡਬੈਕ</t>
         </is>
       </c>
       <c r="L36" t="inlineStr">
@@ -2914,7 +2914,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>এই পৃষ্ঠা সম্পর্কে আপনার কী মতামত?</t>
+          <t>এই পৃষ্ঠা সম্পর্কে আপনার কী মতামত</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
@@ -3034,7 +3034,7 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>नीचे अपना फीडबैक  शेयर करें:</t>
+          <t>नीचे अपना फीडबैक शेयर करें:</t>
         </is>
       </c>
       <c r="D40" t="inlineStr"/>
@@ -3070,7 +3070,7 @@
       </c>
       <c r="K40" t="inlineStr">
         <is>
-          <t>ਆਪਣੀ ਪ੍ਰਤੀਕਿਰਿਆ ਹੇਠਾਂ ਸ਼ੇਅਰ ਕਰੋ:</t>
+          <t>ਆਪਣਾ ਫੀਡਬੈਕ ਹੇਠਾਂ ਸ਼ੇਅਰ ਕਰੋ:</t>
         </is>
       </c>
       <c r="L40" t="inlineStr">
@@ -3113,7 +3113,7 @@
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Would you recommend Bhasha Daan to your friends &amp; family?</t>
+          <t>আপুনি ভাষা দানক আপোনাৰ বন্ধু-বান্ধৱ আৰু পৰিয়ালৰ সদস্য সকলক ব্যৱহাৰ কৰাৰ পৰামৰ্শ দিবনে?</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -3181,7 +3181,7 @@
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Would you revisit Bhasha Daan?</t>
+          <t>আপুনি ভাষা দানলৈ পুনৰ উভটি আহিবনে?</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -3284,7 +3284,7 @@
       </c>
       <c r="M43" t="inlineStr">
         <is>
-          <t>ଇଚ୍ଛାଧିନ</t>
+          <t>ଇଚ୍ଛାଧୀନ</t>
         </is>
       </c>
       <c r="N43" t="inlineStr">
@@ -3342,7 +3342,7 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>*ਲੋੜੀਂਦਾ</t>
+          <t>*ਜ਼ਰੂਰੀ</t>
         </is>
       </c>
       <c r="L44" t="inlineStr">
@@ -3410,7 +3410,7 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>ਕੋਈ ਸ਼੍ਰੇਣੀ ਚੁਣੋ</t>
+          <t>ਇੱਕ ਸ਼੍ਰੇਣੀ ਚੁਣੋ</t>
         </is>
       </c>
       <c r="L45" t="inlineStr">
@@ -3546,7 +3546,7 @@
       </c>
       <c r="K47" t="inlineStr">
         <is>
-          <t>ਗੜਬੜੀ</t>
+          <t>ਗਲਤੀਆਂ</t>
         </is>
       </c>
       <c r="L47" t="inlineStr">
@@ -3725,7 +3725,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>হয়</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
@@ -3793,7 +3793,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>নহয়</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -3861,7 +3861,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Maybe</t>
+          <t>হয়তো</t>
         </is>
       </c>
       <c r="G52" t="inlineStr">
@@ -4362,7 +4362,7 @@
       </c>
       <c r="K59" t="inlineStr">
         <is>
-          <t>ਸਾਰੇ ਫੀਲਡ ਵਿਕਲਪਿਕ ਹਨ ਪਰ ਤੁਸੀਂ ਆਪਣੀ ਜਨ-ਸੰਖਿਆ ਸੰਬੰਧੀ ਜਾਣਕਾਰੀ ਦੇ ਕੇ ਆਪਣੇ ਡਾਟਾ-ਸੈੱਟ ਦੇ ਯੋਗਦਾਨ ਨੂੰ ਵਧਾ ਸਕਦੇ ਹੋ।</t>
+          <t>ਸਾਰੇ ਫੀਲਡ ਵਿਕਲਪਿਕ ਹਨ ਪਰ ਤੁਸੀਂ ਆਪਣੀ ਜਨ-ਸੰਖਿਆ ਸੰਬੰਧੀ ਵੇਰਵਾ ਦੇ ਕੇ ਆਪਣੇ ਡਾਟਾ-ਸੈੱਟ ਦੇ ਯੋਗਦਾਨ ਨੂੰ ਵਧਾ ਸਕਦੇ ਹੋ।</t>
         </is>
       </c>
       <c r="L59" t="inlineStr">
@@ -4530,7 +4530,7 @@
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>उपयोगकर्ता के नाम के लिए ईमेल या फ़ोन नंबर का उपयोग ना करें</t>
+          <t>उपयोगकर्ता के नाम के लिए  ईमेल या फ़ोन नंबर का उपयोग ना करें</t>
         </is>
       </c>
       <c r="D62" t="inlineStr"/>
@@ -4598,58 +4598,58 @@
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>केवल 12 वर्ण संभव (उदाहरण: name.surname, name_surname12 आदि)</t>
+          <t>केवल 12 वर्ण संभव (उदाहरण: name.surname, name_surname आदि)</t>
         </is>
       </c>
       <c r="D63" t="inlineStr"/>
       <c r="E63" t="inlineStr">
         <is>
-          <t>ફક્ત 12 અક્ષરોની અનુમતિ છે. (સૂચન: નામ.અટક, નામ_અટક12 વગેરે)</t>
+          <t>ફક્ત 12 અક્ષરોની અનુમતિ છે. (સૂચન: નામ.અટક, નામ_અટક વગેરે)</t>
         </is>
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>কেৱল ১২ টা বৰ্ণৰ অনুমতি দিয়া হ'ব। (উদাহৰণ: নাম.উপাধি, name_surname12 ইত্যাদি)</t>
+          <t>কেৱল ১২ টা বৰ্ণৰ অনুমতি দিয়া হ'ব। (উদাহৰণ: নাম.উপাধি, name_surname ইত্যাদি)</t>
         </is>
       </c>
       <c r="G63" t="inlineStr">
         <is>
-          <t>শুধুমাত্র ১২টি অক্ষর অনুমোদিত। (সাহায্যপূর্ণ সংকেত: নাম.পদবী, নাম_পদবী ১২  ইত্যাদি)</t>
+          <t>শুধুমাত্র ১২টি অক্ষর অনুমোদিত। (সাহায্যপূর্ণ সংকেত: নাম.পদবী, নাম_পদবী  ইত্যাদি)</t>
         </is>
       </c>
       <c r="H63" t="inlineStr">
         <is>
-          <t>12 எழுத்துக்கள் மட்டுமே அனுமதிக்கப்படுகின்றன. (குறிப்பு: பெயர்.குடும்பப்பெயர்,பெயர்_குடும்பப்பெயர்12 போன்றவை)</t>
+          <t>12 எழுத்துக்கள் மட்டுமே அனுமதிக்கப்படுகின்றன. (குறிப்பு: பெயர்.குடும்பப்பெயர்,பெயர்_குடும்பப்பெயர் போன்றவை)</t>
         </is>
       </c>
       <c r="I63" t="inlineStr">
         <is>
-          <t>12 అక్షరాలు మాత్రమే ఉండాలి. (ఉదా: name.surname, name_surname12 etc.)</t>
+          <t>12 అక్షరాలు మాత్రమే ఉండాలి. (ఉదా: name.surname, name_surname etc.)</t>
         </is>
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>फक्त १२ वर्णांची संभावना. (टिप : name.surname, name_surname12 etc..)</t>
+          <t>फक्त १२ वर्णांची संभावना. (टिप : name.surname, name_surname etc..)</t>
         </is>
       </c>
       <c r="K63" t="inlineStr">
         <is>
-          <t>ਸਿਰਫ 12 ਅੱਖਰਾਂ ਦੀ ਇਜਾਜ਼ਤ ਹੈ। (ਜਿਵੇਂ : name.surname, name_surname12 ਆਦਿ)</t>
+          <t>ਸਿਰਫ 12 ਅੱਖਰਾਂ ਦੀ ਇਜਾਜ਼ਤ ਹੈ। (ਜਿਵੇਂ : ਨਾਮ.ਸਰਨੇਮ, ਨਾਮ_ਸਰਨੇਮ ਆਦਿ)</t>
         </is>
       </c>
       <c r="L63" t="inlineStr">
         <is>
-          <t>12 പ്രതീകങ്ങൾ മാത്രമേ അനുവദിച്ചിട്ടുള്ളൂ. (സൂചന: name.surname, name_surname12 മുതലായവ)</t>
+          <t>12 പ്രതീകങ്ങൾ മാത്രമേ അനുവദിച്ചിട്ടുള്ളൂ. (സൂചന: name.surname, name_surname മുതലായവ)</t>
         </is>
       </c>
       <c r="M63" t="inlineStr">
         <is>
-          <t>କେବଳ 12 ଅକ୍ଷର ହିଁ ସମ୍ଭବ (ଉଦାହରଣ: name.surname, name_surname12 ଇତ୍ୟାଦି)</t>
+          <t>କେବଳ 12 ଅକ୍ଷର ହିଁ ସମ୍ଭବ (ଉଦାହରଣ: name.surname, name_surname ଇତ୍ୟାଦି)</t>
         </is>
       </c>
       <c r="N63" t="inlineStr">
         <is>
-          <t>ಕೇವಲ 12 ಅಕ್ಷರಗಳನ್ನು ಮಾತ್ರ ಕೊಡಲು ಸಾಧ್ಯ. (ಸುಳಿವು: ಹೆಸರು.ಅಡ್ಡಹೆಸರು, ಹೆಸರು_ಅಡ್ಡಹೆಸರು12 ಇತ್ಯಾದಿ)</t>
+          <t>ಕೇವಲ 12 ಅಕ್ಷರಗಳನ್ನು ಮಾತ್ರ ಕೊಡಲು ಸಾಧ್ಯ. (ಸುಳಿವು: ಹೆಸರು.ಅಡ್ಡಹೆಸರು, ಹೆಸರು_ಅಡ್ಡಹೆಸರು ಇತ್ಯಾದಿ)</t>
         </is>
       </c>
     </row>
@@ -5795,12 +5795,12 @@
       </c>
       <c r="L80" t="inlineStr">
         <is>
-          <t>ഭിന്നലിംഗം-അവൻ</t>
+          <t>ഭിന്നലിംഗം- അവൻ</t>
         </is>
       </c>
       <c r="M80" t="inlineStr">
         <is>
-          <t>ଟ୍ରାନ୍ସଜେଣ୍ଡର - ସେ (ପୁରୁଷ)</t>
+          <t>ଟ୍ରାନ୍ସଜେଣ୍ଡର - ପୁରୁଷ</t>
         </is>
       </c>
       <c r="N80" t="inlineStr">
@@ -5863,12 +5863,12 @@
       </c>
       <c r="L81" t="inlineStr">
         <is>
-          <t>ഭിന്നലിംഗം-അവൾ</t>
+          <t>ഭിന്നലിംഗം- അവൾ</t>
         </is>
       </c>
       <c r="M81" t="inlineStr">
         <is>
-          <t>ଟ୍ରାନ୍ସଜେଣ୍ଡର - ସେ (ମହିଳା)</t>
+          <t>ଟ୍ରାନ୍ସଜେଣ୍ଡର - ମହିଳା</t>
         </is>
       </c>
       <c r="N81" t="inlineStr">
@@ -5969,7 +5969,7 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Not Specified</t>
+          <t>নিৰ্দিষ্ট কৰা নাই</t>
         </is>
       </c>
       <c r="G83" t="inlineStr">
@@ -5994,7 +5994,7 @@
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>ਨਹੀਂ ਦਰਸਾਇਆ</t>
+          <t>ਦਿੱੱਤਾ ਨਹੀਂ</t>
         </is>
       </c>
       <c r="L83" t="inlineStr">
@@ -6118,7 +6118,7 @@
       </c>
       <c r="K86" t="inlineStr">
         <is>
-          <t>ਸਮਾਪਤ</t>
+          <t>ਮੁਕੰਮਲ</t>
         </is>
       </c>
       <c r="L86" t="inlineStr">
@@ -6214,7 +6214,7 @@
       </c>
       <c r="K88" t="inlineStr">
         <is>
-          <t>ਗੋਪਨੀਯਤਾ ਨੀਤੀ</t>
+          <t>ਪ੍ਰਾਈਵੇਸੀ ਨੀਤੀ</t>
         </is>
       </c>
       <c r="L88" t="inlineStr">
@@ -6262,7 +6262,7 @@
       </c>
       <c r="G89" t="inlineStr">
         <is>
-          <t>আপনার পরিবার এবং বন্ধুদের কে এটিতে অংশী হতে নিমন্ত্রণ করুন</t>
+          <t>আপনার পরিবার এবং বন্ধুদেরকে এটিতে অংশী হতে নিমন্ত্রণ করুন</t>
         </is>
       </c>
       <c r="H89" t="inlineStr">
@@ -6282,7 +6282,7 @@
       </c>
       <c r="K89" t="inlineStr">
         <is>
-          <t>ਆਪਣੇ ਦੋਸਤਾਂ ਅਤੇ ਪਰਿਵਾਰਕ ਮੈਂਬਰਾਂ ਨਾਲ ਸ਼ੇਅਰ ਕਰੋ</t>
+          <t>ਆਪਣੇ ਦੋਸਤਾਂ ਅਤੇ ਪਰਿਵਾਰਕ ਮੈਂਬਰਾਂ ਦੇ ਨਾਲ ਸ਼ੇਅਰ ਕਰੋ</t>
         </is>
       </c>
       <c r="L89" t="inlineStr">
@@ -6314,58 +6314,58 @@
       </c>
       <c r="C90" t="inlineStr">
         <is>
-          <t>मैंने  https://bhashini.gov.in/bhashadaan पर भारत के लिए ओपन लैंग्वेज रिपोजिटरी बनाने में योगदान दिया है। हम और आप भाषा दान में योगदान देकर एक बदलाव ला सकते हैं जो मशीनों को हमारी भाषा सीखने और अच्छी भाषाई एप्लिकेशन्स के माध्यम से हमारे साथ संपर्क करने में मदद कर सकता है। अपना योगदान दें और भाषा को सशक्त बनाएं।</t>
+          <t>मैंने https://bhashini.gov.in/bhasadaan पर भारत के लिए ओपन लैंग्वेज रिपोजिटरी बनाने में योगदान दिया है। आइए भाषा दान में योगदान देकर बदलाव लाएं और अपनी अपनी भाषाओं को सशक्त बनाएं।</t>
         </is>
       </c>
       <c r="D90" t="inlineStr"/>
       <c r="E90" t="inlineStr">
         <is>
-          <t>મેં https://bhashini.gov.in/bhashadaan પર ભારત માટે ઓપન ભાષા ભંડાર બનાવવા માટે ફાળો આપ્યો છે. તમે અને હું ભાષા દાનમાં યોગદાન આપીને તફાવત લાવી શકીએ છીએ જે મશીનોને આપણી ભાષા શીખવામાં મદદ કરી શકશે અને વિવિધ લિંગ્વિસ્ટીક એપ્લિકેશન દ્વારા આપણી સાથે સંપર્ક કરી શકશે. તમારું યોગદાન આપો અને ભાષાને સશક્ત બનાવો</t>
+          <t>મેં https://bhashini.gov.in/bhasadaan પર ભારત માટે ઓપન લેંગ્વેજ રિપોઝીટરી બનાવવા માટે યોગદાન આપ્યું છે. ચાલો ભાષા દાનમાં યોગદાન આપીને આપણી ભાષાઓને સશક્ત બનાવીએ.</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>মই https://bhashini.gov.in/bhashadaan ত ভাৰতৰ বাবে মুক্ত ভাষাৰ ভাণ্ডাৰ নিৰ্মাণত অবদান আগবঢ়াইছো৷ আপুনি আৰু মই আমাৰ কণ্ঠদান কৰি এটা পাৰ্থক্য সৃষ্টি কৰিব পাৰোঁ যিয়ে যন্ত্ৰবোৰক আমাৰ ভাষা শিকিবলৈ সহায় কৰিব পাৰে। আপোনাৰ অংশটো কৰি ভাষাটো শক্তিশালী কৰক?</t>
+          <t>মই ভাৰতৰ বাবে মুক্ত ভাষা ভঁৰাল সাজিবলৈ https://bhashini.gov.in/bhashadaan ত অৰিহণা আগবঢ়াইছো৷ ভাষা দানত অৰিহণা আগবঢ়াই এটা পাৰ্থক্যৰ সৃষ্টি আৰু আমাৰ ভাষাসমূহক শক্তিশালী কৰি তোলো আহক৷</t>
         </is>
       </c>
       <c r="G90" t="inlineStr">
         <is>
-          <t>https://bhashini.gov.in/bhashadaan এ আমি ভারতের জন্য উন্মুক্ত ভাষা ভাণ্ডার তৈরির ক্ষেত্রে যোগদান দিয়েছি। আপনি এবং আমি ভাষা দান এ যোগদানের মাধ্যমে একটি পার্থক্য তৈরি করতে পারি যা মেশিনগুলিকে আমাদের ভাষা শিখতে এবং দুর্দান্ত ভাষাগত প্রয়োগের মাধ্যমে আমাদের সাথে যোগাযোগ করতে সহায়তা করতে পারে। আপনার স্বল্প যোগদান দিয়ে ভাষাটিকে ক্ষমতাশীল করুন ।</t>
+          <t>ভারতের ওপেন ল্যাঙ্গুয়েজ রিপোজিটরি তৈরিতে আমি https://bhashini.gov.in/bhasadaan - তে  অবদান রেখেছি। আসুন ভাষাদান এ যোগদান করে একটি ভিন্নতা তৈরি করি এবং আমাদের ভাষাকে শক্তিশালী করি।</t>
         </is>
       </c>
       <c r="H90" t="inlineStr">
         <is>
-          <t>Https://bhashini.gov.in/bhashadaan இல் இந்தியாவிற்கான திறந்த மொழி களஞ்சியத்தை உருவாக்க நான் பங்களித்திருக்கிறேன். நீங்களும் நானும் பாஷா டானுக்கு பங்களிப்பதன் மூலம் ஒரு வித்தியாசத்தை உருவாக்க முடியும், இது இயந்திரங்கள் நம் மொழியைக் கற்றுக்கொள்ள உதவுகிறது மற்றும் சிறந்த மொழியியல் பயன்பாடுகளின் மூலம் எங்களுடன் தொடர்பு கொள்ள முடியும். உங்கள் பிட் மற்றும் மொழியை மேம்படுத்துகிறீர்களா?</t>
+          <t>இந்தியாவிற்கான திறந்த மொழி களஞ்சியத்தை உருவாக்க நான் https://bhashini.gov.in/bhashadaan இல் பங்களித்துள்ளேன். பாஷா தானுக்கு பங்களிப்பதன் மூலம் ஒரு வித்தியாசத்தை ஏற்படுத்துவோம் மற்றும் நம் மொழிகளுக்கு அதிகாரம் அளிப்போம்.</t>
         </is>
       </c>
       <c r="I90" t="inlineStr">
         <is>
-          <t>Https://bhashini.gov.in/bhashadaan లో భారతదేశం కోసం ఓపెన్ లాంగ్వేజ్ రిపోజిటరీని నిర్మించటానికి నేను కాంట్రిబ్యూట్ చేసాను. భాషా దాన్‌కు కాంట్రిబ్యూట్ చేయడం ద్వారా మీరు మరియు మేము ఒక మార్పును తేగలము, యంత్రాలు మన భాషను నేర్చుకోవటానికి మరియు ఉత్తమ భాషా అనువర్తనాల ద్వారా మనతో సంభాషించడానికి ఇది సహాయపడుతుంది. మీరు కాంట్రిబ్యూట్ చేసి మరియు భాషకు సాధికారతను చేకూర్చండి.</t>
+          <t>నేను భారతదేశం కోసం https://bhashini.gov.in/bhashadaan లో ఓపెన్ లాంగ్వేజ్ రిపోజిటరీని నిర్మించడానికి కాంట్రిబ్యూట్ చేసాను. భాషా దాన్‌లో కాంట్రిబ్యూట్ చేసి మన భాషలను శక్తివంతం చేయడం ద్వారా ఒక వైవిధ్యాన్ని చూద్దాం.</t>
         </is>
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>मी https://bhashini.gov.in/bhashadaan वर भारतासाठी ओपन लॅंग्वेज रिपोझिटरीच्या उभारणीस योगदान दिले आहे. आपण आणि मी भाषा दानात योगदान देवून एक बदलाव आणू शकतो ज्यामुळे मशीन आपली भाषा शिकण्यास  आणि उत्कृष्ट भाषिक अनुप्रयोगांद्वारे आमच्याशी संवाद साधण्यास मदत करू शकाल. आपले योगदान देऊन भाषा सक्षम करा.</t>
+          <t>मी https://bhashini.gov.in/bhashadaan वर भारतासाठी मुक्त भाषा भांडार तयार करण्यासाठी योगदान दिले आहे. भाषा दानामध्ये योगदान देऊन आणि आपल्या भाषांना सक्षम बनवून एक बदल घडवून आणूया.</t>
         </is>
       </c>
       <c r="K90" t="inlineStr">
         <is>
-          <t>ਮੈਂ https://bhashini.gov.in/bhashadaan 'ਤੇ ਭਾਰਤ ਲਈ ਓਪਨ ਲੈਂਗੁਏਜ ਰਿਪੋਜ਼ਿਟਰੀ ਬਣਾਉਣ ਵਿੱਚ ਯੋਗਦਾਨ ਪਾਇਆ ਹੈ। ਤੁਸੀਂ ਅਤੇ ਮੈਂ ਭਾਸ਼ਾ ਦਾਨ ਵਿਚ ਯੋਗਦਾਨ ਪਾ ਕੇ ਤਬਦੀਲੀ ਲਿਆ ਸਕਦੇ ਹਾਂ ਜੋ ਮਸ਼ੀਨਾਂ ਨੂੰ ਸਾਡੀ ਭਾਸ਼ਾ ਸਿੱਖਣ ਅਤੇ  ਮਹਾਨ ਭਾਸ਼ਾਈ ਐਪਲੀਕੇਸ਼ਨਾਂ ਰਾਹੀਂ ਸਾਡੇ ਨਾਲ ਗੱਲਬਾਤ ਕਰਨ ਵਿੱਚ ਮਦਦ ਕਰ ਸਕਦਾ ਹੈ। ਆਪਣਾ ਕੰਮ ਕਰੋ ਅਤੇ ਭਾਸ਼ਾ ਨੂੰ ਪ੍ਰਭਾਵਸ਼ਾਲੀ ਬਣਾਓ</t>
+          <t>ਮੈਂ https://bhashini.gov.in/bhasadaan 'ਤੇ ਭਾਰਤ ਦੇ ਲਈ ਓਪਨ ਲੈਂਗੁਏਜ ਰਿਪੋਜ਼ਿਟਰੀ ਬਣਾਉਣ ਵਿੱਚ ਯੋਗਦਾਨ ਪਾਇਆ ਹੈ। ਆਓ ਭਾਸ਼ਾ ਦਾਨ ਵਿੱਚ ਯੋਗਦਾਨ ਪਾ ਕੇ ਇੱਕ ਬਦਲਾਅ ਲਿਆਈਏ ਅਤੇ ਆਪਣੀਆਂ ਭਾਸ਼ਾਵਾਂ ਨੂੰ ਸ਼ਕਤੀਸ਼ਾਲੀ ਬਣਾਈਏ।</t>
         </is>
       </c>
       <c r="L90" t="inlineStr">
         <is>
-          <t>ഇന്ത്യയ്‌ക്കായി ഓപ്പൺ ലാംഗ്വേജ് ശേഖരം നിർമ്മിക്കുന്നതിന്  https://bhashini.gov.in/bhashadaan -ൽ ഞാൻ സംഭാവന നൽകി.  മികച്ച ഭാഷാ ആപ്ലിക്കേഷനുകളിലൂടെ നമ്മുടെ ഭാഷ പഠിക്കാനും നമ്മളുമായി സംവദിക്കാനും യന്ത്രങ്ങളെ സഹായിക്കുന്ന ഭാഷാ ദാനിലേക്ക് സംഭാവന ചെയ്യുന്നതിലൂടെ നിങ്ങൾക്കും എനിക്കും ഒരു മാറ്റമുണ്ടാക്കാൻ കഴിയും.</t>
+          <t>ഇന്ത്യയ്ക്കായി ഒരു തുറന്ന ഭാഷാ ശേഖരം നിർമ്മിക്കുന്നതിന് https://bhashini.gov.in/bhashadaan -ൽ ഞാൻ സംഭാവന നൽകി. ഭാഷാ ദാനിൽ സംഭാവന നല്കുന്നതിലൂടെ ഒരു മാറ്റമുണ്ടാക്കുകയും നമ്മുടെ ഭാഷകളെ ശാക്തീകരിക്കുകയും ചെയ്യാം.</t>
         </is>
       </c>
       <c r="M90" t="inlineStr">
         <is>
-          <t>ମୁଁ https://bhashini.gov.in/bhashadaan ରେ ଭାରତ ପାଇଁ ଏକ ଓପନ ଲାଙ୍ଗୁଏଜ ରିପୋଜିଟରି ନିର୍ମାଣ କରିବା ଦିଗରେ ଯୋଗଦାନ କରିଛି । ଆମେ ଭାଷା ଦାନରେ ଯୋଗ ଦେଇ ଏକ ପରିବର୍ତ୍ତନ ଆଣିପାରିବା ଯାହାକି ମେସିନଗୁଡ଼ିକୁ ଆମ ଭାଷାକୁ ଶିଖିବାରେ ଓ ଅନେକ ଭାଷା ସମ୍ବଧୀୟ ପ୍ରୟୋଗ ମାଧ୍ୟମରେ ଆମ ସହିତ ସମ୍ପର୍କ ସ୍ଥାପନ କରିବାରେ ସାହାଯ୍ୟ କରିବ।  ଯୋଗଦାନ କରି ନିଜର ଭାଷାକୁ ଆହୁରି ସଶକ୍ତ କରନ୍ତୁ।</t>
+          <t>ମୁଁ https://bhashini.gov.in/bhashadaan ରେ ଭାରତ ପାଇଁ ଏକ ଓପନ ଲାଙ୍ଗୁଏଜ ରିପୋଜିଟରୀ ତିଆରି କରିବା ଦିଗରେ ଯୋଗଦାନ କରିଛି। ଆସନ୍ତୁ, ଭାଷା ଦାନରେ ଯୋଗଦାନ କରି ଏକ ନୂତନ ପରିବର୍ତ୍ତନରେ ସାମିଲ ହେବା ଓ ଆମ ଭାଷାଗୁଡ଼ିକୁ ସମୃଦ୍ଧ କରିବା।</t>
         </is>
       </c>
       <c r="N90" t="inlineStr">
         <is>
-          <t>https://bhashini.gov.in/bhashadaan ನಲ್ಲಿ ಭಾರತಕ್ಕಾಗಿ ಒಂದು ಓಪನ್ ಲ್ಯಾಂಗ್ವೇಜ್ ರೆಪಾಸಿಟರಿಯನ್ನು ನಿರ್ಮಿಸಲು ನಾನು ಕೊಡುಗೆ ನೀಡಿದ್ದೇನೆ. ಭಾಷಾ ದಾನ್‌ಗೆ ಕೊಡುಗೆ ನೀಡುವ ಮೂಲಕ ನಾವು ನೀವು ಸೇರಿ ಒಂದು ವ್ಯತ್ಯಾಸವನ್ನು ತರಬಹುದು. ಯಂತ್ರಗಳು ನಮ್ಮ ಭಾಷೆಯನ್ನು ಕಲಿಯಲು ಮತ್ತು ಉತ್ತಮ ಭಾಷಾ ಅನ್ವಯಗಳ ಮೂಲಕ ನಮ್ಮೊಂದಿಗೆ ಸಂವಹನ ನಡೆಸಲು ಇದು ಸಹಾಯ ಮಾಡುತ್ತದೆ. ನಿಮ್ಮ ಕೊಡುಗೆಯನ್ನು ನೀಡಿ ಭಾಷೆಯನ್ನು ಸಮೃದ್ಧಗೊಳಿಸಿ.</t>
+          <t>ನಾನು https://bhashini.gov.in/bhashadaan ನಲ್ಲಿ ಭಾರತಕ್ಕಾಗಿ ಮುಕ್ತ ಭಾಷಾ ಭಂಡಾರವನ್ನು ನಿರ್ಮಿಸಲು ಕೊಡುಗೆ ನೀಡಿದ್ದೇನೆ. ಭಾಷಾ ದಾನಕ್ಕೆ ಕೊಡುಗೆ ನೀಡುವ ಮೂಲಕ ಮತ್ತು ನಮ್ಮ ಭಾಷೆಗಳನ್ನು ಸಬಲೀಕರಣಗೊಳಿಸುವ ಮೂಲಕ ಒಂದು ವ್ಯತ್ಯಾಸವನ್ನು ತರೋಣ.</t>
         </is>
       </c>
     </row>
@@ -6546,58 +6546,58 @@
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>फीडबैक देने के लिए धन्यवाद</t>
+          <t>फीडबैक देने के लिए धन्यवाद!</t>
         </is>
       </c>
       <c r="D96" t="inlineStr"/>
       <c r="E96" t="inlineStr">
         <is>
-          <t>આપના પ્રતિભાવ બદલ આભાર</t>
+          <t>આપના પ્રતિભાવ બદલ આભાર!</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>আপোনাৰ মতামতৰ বাবে আপোনাক ধন্যবাদ</t>
+          <t>আপোনাৰ মতামতৰ বাবে আপোনাক ধন্যবাদ!</t>
         </is>
       </c>
       <c r="G96" t="inlineStr">
         <is>
-          <t>আপনার মতামতের জন্য ধন্যবাদ</t>
+          <t>আপনার মতামতের জন্য ধন্যবাদ!</t>
         </is>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>உங்கள் கருத்திற்கு நன்றி</t>
+          <t>உங்கள் கருத்திற்கு நன்றி!</t>
         </is>
       </c>
       <c r="I96" t="inlineStr">
         <is>
-          <t>మీ అభిప్రాయం తెలియజేసినందుకు ధన్యవాదములు</t>
+          <t>మీ అభిప్రాయం తెలియజేసినందుకు ధన్యవాదములు!</t>
         </is>
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>आपल्या अभिप्रायाबद्दल धन्यवाद</t>
+          <t>आपल्या अभिप्रायाबद्दल धन्यवाद!</t>
         </is>
       </c>
       <c r="K96" t="inlineStr">
         <is>
-          <t>ਫੀਡਬੈਕ ਦੇ ਲਈ ਤੁਹਾਡਾ ਸ਼ੁਕਰੀਆ</t>
+          <t>ਫੀਡਬੈਕ ਦੇ ਲਈ ਤੁਹਾਡਾ ਸ਼ੁਕਰੀਆ!</t>
         </is>
       </c>
       <c r="L96" t="inlineStr">
         <is>
-          <t>നിങ്ങളുടെ അഭിപ്രായത്തിന് നന്ദി</t>
+          <t>നിങ്ങളുടെ അഭിപ്രായത്തിന് നന്ദി!</t>
         </is>
       </c>
       <c r="M96" t="inlineStr">
         <is>
-          <t>ଆପଣଙ୍କ ଫିଡବ୍ୟାକ ପାଇଁ ଧନ୍ୟବାଦ</t>
+          <t>ଆପଣଙ୍କ ଫିଡବ୍ୟାକ ପାଇଁ ଧନ୍ୟବାଦ!</t>
         </is>
       </c>
       <c r="N96" t="inlineStr">
         <is>
-          <t>ನಿಮ್ಮ ಪ್ರತಿಕ್ರಿಯೆಯನ್ನು ನೀಡಿದ್ದಕ್ಕಾಗಿ ಧನ್ಯವಾದಗಳು</t>
+          <t>ನಿಮ್ಮ ಪ್ರತಿಕ್ರಿಯೆಯನ್ನು ನೀಡಿದ್ದಕ್ಕಾಗಿ ಧನ್ಯವಾದಗಳು!</t>
         </is>
       </c>
     </row>
@@ -6897,7 +6897,7 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Overall Summary</t>
+          <t>সামগ্ৰিক সাৰাংশ</t>
         </is>
       </c>
       <c r="G101" t="inlineStr">
@@ -6965,7 +6965,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Only contributions invited for the selected language</t>
+          <t>মাত্ৰ বাচি লোৱা ভাষাৰ বাবে মাত্ৰ অৰিহনা আমন্ত্ৰিত</t>
         </is>
       </c>
       <c r="G102" t="inlineStr">
@@ -6990,7 +6990,7 @@
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>ਸਿਰਫ ਚੁੁਣੀ ਗਈ ਭਾਸ਼ਾ ਦੇ ਲਈ ਹੀ ਯੋਗਦਾਨ ਦਾ ਸੱਦਾ</t>
+          <t>ਚੁੁਣੀ ਗਈ ਭਾਸ਼ਾ ਦੇ ਲਈ ਹੀ ਸਿਰਫ ਯੋਗਦਾਨ ਦਾ ਸੱਦਾ</t>
         </is>
       </c>
       <c r="L102" t="inlineStr">
@@ -7033,7 +7033,7 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Only validations invited for the selected language</t>
+          <t>মাত্ৰ বাচি লোৱা ভাষাৰ বাবে মাত্ৰ বৈধতা প্ৰদান আমন্ত্ৰিত</t>
         </is>
       </c>
       <c r="G103" t="inlineStr">
@@ -7058,7 +7058,7 @@
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>ਸਿਰਫ ਚੁਣੀ ਗਈ ਭਾਸ਼ਾ ਦੇ ਲਈ ਹੀ ਪ੍ਰਮਾਣੀਕਰਨ ਦਾ ਸੱਦਾ</t>
+          <t>ਚੁਣੀ ਗਈ ਭਾਸ਼ਾ ਦੇ ਲਈ ਹੀ ਸਿਰਫ ਪ੍ਰਮਾਣੀਕਰਨ ਦਾ ਸੱਦਾ</t>
         </is>
       </c>
       <c r="L103" t="inlineStr">
@@ -7194,7 +7194,7 @@
       </c>
       <c r="K105" t="inlineStr">
         <is>
-          <t>ਆਪਣੀ ਆਵਾਜ਼ ਦਾ ਯੋਗਦਾਨ ਪਾਓ</t>
+          <t>ਆਵਾਜ਼ ਦਾ ਯੋਗਦਾਨ ਦਿਓ</t>
         </is>
       </c>
       <c r="L105" t="inlineStr">
@@ -7226,7 +7226,7 @@
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>इमेज में दिए  गए  टेक्स्ट को टाइप करें</t>
+          <t>इमेज में दिए गए टेक्स्ट को टाइप करें</t>
         </is>
       </c>
       <c r="D106" t="inlineStr"/>
@@ -7373,7 +7373,7 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>ছৱি অনুযায়ী আনে লেবেল লগোৱা পাঠ বৈধকৰণ কৰক</t>
+          <t>আন লোকসকলে আগবঢ়োৱা অৰিহণাক বৈধতা প্ৰদান কৰক</t>
         </is>
       </c>
       <c r="G108" t="inlineStr">
@@ -7441,7 +7441,7 @@
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>ছৱি অনুযায়ী আনে লেবেল লগোৱা পাঠ বৈধকৰণ কৰক</t>
+          <t>আন লোকসকলে আগবঢ়োৱা অৰিহণাক বৈধতা প্ৰদান কৰক</t>
         </is>
       </c>
       <c r="G109" t="inlineStr">
@@ -7509,7 +7509,7 @@
       </c>
       <c r="F110" t="inlineStr">
         <is>
-          <t>ছৱি অনুযায়ী আনে লেবেল লগোৱা পাঠ বৈধকৰণ কৰক</t>
+          <t>আন লোকসকলে আগবঢ়োৱা অৰিহণাক বৈধতা প্ৰদান কৰক</t>
         </is>
       </c>
       <c r="G110" t="inlineStr">
@@ -7577,7 +7577,7 @@
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>ছৱি অনুযায়ী আনে লেবেল লগোৱা পাঠ বৈধকৰণ কৰক</t>
+          <t>আন লোকসকলে আগবঢ়োৱা অৰিহণাক বৈধতা প্ৰদান কৰক</t>
         </is>
       </c>
       <c r="G111" t="inlineStr">
@@ -7645,7 +7645,7 @@
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>Month</t>
+          <t>মাহ</t>
         </is>
       </c>
       <c r="G112" t="inlineStr">
@@ -7713,7 +7713,7 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>Contribution (in hours)</t>
+          <t>অৱদান (ঘন্টাত)</t>
         </is>
       </c>
       <c r="G113" t="inlineStr">
@@ -7781,7 +7781,7 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>Contribution (in hours)</t>
+          <t>অৱদান (ঘন্টাত)</t>
         </is>
       </c>
       <c r="G114" t="inlineStr">
@@ -7849,7 +7849,7 @@
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>Contribution (total translations)</t>
+          <t>অৰিহনা (মুঠ অনুবাদ)</t>
         </is>
       </c>
       <c r="G115" t="inlineStr">
@@ -7917,7 +7917,7 @@
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>Contribution (total images)</t>
+          <t>অৰিহনা (মুঠ ছবি)</t>
         </is>
       </c>
       <c r="G116" t="inlineStr">
@@ -7985,7 +7985,7 @@
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>Contribution (total speakers)</t>
+          <t>অৰিহনা (মুঠ বক্তা)</t>
         </is>
       </c>
       <c r="G117" t="inlineStr">
@@ -8053,7 +8053,7 @@
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>Contribution (total sentences)</t>
+          <t>অৰিহনা (মুঠ বাক্য)</t>
         </is>
       </c>
       <c r="G118" t="inlineStr">
@@ -8189,7 +8189,7 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>Transcription (in sentences)</t>
+          <t>প্ৰতিলিপিকৰণ (বাক্যবোৰত)</t>
         </is>
       </c>
       <c r="G120" t="inlineStr">
@@ -8199,7 +8199,7 @@
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>எடுத்தெழுதுதல் (வாக்கியங்களில்)</t>
+          <t>டிரான்ஸ்க்ரிப்ஷன் (வாக்கியங்களில்)</t>
         </is>
       </c>
       <c r="I120" t="inlineStr">
@@ -8214,7 +8214,7 @@
       </c>
       <c r="K120" t="inlineStr">
         <is>
-          <t>ਲਿਪੀਅੰਤਰਣ (ਵਾਕਾਂ ਵਿਚ)</t>
+          <t>ਟ੍ਰਾਂਸਕ੍ਰਿਪਸ਼ਨ (ਵਾਕਾਂ ਵਿਚ)</t>
         </is>
       </c>
       <c r="L120" t="inlineStr">
@@ -8325,7 +8325,7 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>Translation (in sentences)</t>
+          <t>অনুবাদ (বাক্যত)</t>
         </is>
       </c>
       <c r="G122" t="inlineStr">
@@ -8461,7 +8461,7 @@
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>Validation (in sentences)</t>
+          <t>বৈধতা প্ৰদান( বাক্যত)</t>
         </is>
       </c>
       <c r="G124" t="inlineStr">
@@ -8597,7 +8597,7 @@
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>Validation (in sentences)</t>
+          <t>বৈধতা প্ৰদান( বাক্যত)</t>
         </is>
       </c>
       <c r="G126" t="inlineStr">
@@ -8748,7 +8748,7 @@
       </c>
       <c r="I128" t="inlineStr">
         <is>
-          <t>కాంట్రిబ్యూషన్ చేయడం కోసం భాషను ఎంచుకోండి</t>
+          <t>కాంట్రిబ్యూషన్ చేయడం కోసం భాషా జతను ఎంచుకోండి</t>
         </is>
       </c>
       <c r="J128" t="inlineStr">
@@ -8929,7 +8929,7 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>কোৱা ইণ্ডিয়া লক্ষ্যৰ &lt;গড়&gt;% উপনীত হৈছে</t>
+          <t>কোৱা ইণ্ডিয়া লক্ষ্যৰ &lt;span&gt;{{average}}%&lt;/span&gt; উপনীত হৈছে</t>
         </is>
       </c>
       <c r="G131" t="inlineStr">
@@ -8997,7 +8997,7 @@
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>শুনা ইণ্ডিয়া লক্ষ্যৰ &lt;গড়&gt;% উপনীত হৈছে</t>
+          <t>শুনা ইণ্ডিয়া লক্ষ্যৰ &lt;span&gt;{{average}}%&lt;/span&gt; উপনীত হৈছে</t>
         </is>
       </c>
       <c r="G132" t="inlineStr">
@@ -9065,7 +9065,7 @@
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>চোৱা ইণ্ডিয়া লক্ষ্যৰ &lt;গড়&gt;% উপনীত হৈছে</t>
+          <t>চোৱা ইণ্ডিয়া লক্ষ্যৰ &lt;span&gt;{{average}}%&lt;/span&gt; উপনীত হৈছে</t>
         </is>
       </c>
       <c r="G133" t="inlineStr">
@@ -9133,7 +9133,7 @@
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>লিখা ইণ্ডিয়া লক্ষ্যৰ &lt;গড়&gt;% উপনীত হৈছে</t>
+          <t>লিখা ইণ্ডিয়া লক্ষ্যৰ &lt;span&gt;{{average}}%&lt;/span&gt; উপনীত হৈছে</t>
         </is>
       </c>
       <c r="G134" t="inlineStr">
@@ -9201,7 +9201,7 @@
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>&lt;ভাষা&gt;ৰ &lt;গড়&gt;% কোৱা ইণ্ডিয়া লক্ষ্যত উপনীত হৈছে৷</t>
+          <t>{{language}}ৰ &lt;span&gt;{{average}}%&lt;/span&gt; কোৱা ইণ্ডিয়া লক্ষ্যত উপনীত হৈছে৷</t>
         </is>
       </c>
       <c r="G135" t="inlineStr">
@@ -9269,7 +9269,7 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>&lt;ভাষা&gt;ৰ &lt;গড়&gt;% শুনা ইণ্ডিয়া লক্ষ্যত উপনীত হৈছে৷</t>
+          <t>{{language}}ৰ &lt;span&gt;{{average}}%&lt;/span&gt; শুনা ইণ্ডিয়া লক্ষ্যত উপনীত হৈছে৷</t>
         </is>
       </c>
       <c r="G136" t="inlineStr">
@@ -9337,7 +9337,7 @@
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>&lt;ভাষা&gt;ৰ &lt;গড়&gt;% চোৱা ইণ্ডিয়া লক্ষ্যত উপনীত হৈছে৷</t>
+          <t>{{language}}ৰ &lt;span&gt;{{average}}%&lt;/span&gt; চোৱা ইণ্ডিয়া লক্ষ্যত উপনীত হৈছে৷</t>
         </is>
       </c>
       <c r="G137" t="inlineStr">
@@ -9405,7 +9405,7 @@
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>&lt;ভাষাৰ-পৰা&gt;-&lt;ভাষা-লৈ&gt;ৰ &lt;গড়&gt;% লিকা ইণ্ডিয়া লক্ষ্যত উপনীত হৈছে৷</t>
+          <t>{{language}} ৰ &lt;span&gt;{{average}}%&lt;/span&gt; লিকা ইণ্ডিয়া লক্ষ্যত উপনীত হৈছে৷</t>
         </is>
       </c>
       <c r="G138" t="inlineStr">
@@ -9542,7 +9542,7 @@
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>भाषा दान: भारतीय भाषाओं के लिए एक क्राउडसोर्सिंग पहल</t>
+          <t>भाषा दान: भारतीय भाषाओं के लिए एक क्राउडसोर्सिंग उपक्रम</t>
         </is>
       </c>
       <c r="D142" t="inlineStr"/>
@@ -9563,7 +9563,7 @@
       </c>
       <c r="H142" t="inlineStr">
         <is>
-          <t>மொழி நன்கொடை: இந்திய மொழிகளுக்கான கூட்டசேகரம் முயற்சி</t>
+          <t>பாஷா தான்: இந்திய மொழிகளுக்கான கூட்டசேகரம் முயற்சி</t>
         </is>
       </c>
       <c r="I142" t="inlineStr">
@@ -9755,7 +9755,7 @@
       </c>
       <c r="H146" t="inlineStr">
         <is>
-          <t>எடுத்தெழுத காலஅளவு</t>
+          <t>டிரான்ஸ்க்ரைப்டு காலஅளவு</t>
         </is>
       </c>
       <c r="I146" t="inlineStr">
@@ -9770,7 +9770,7 @@
       </c>
       <c r="K146" t="inlineStr">
         <is>
-          <t>ਲਿਪੀਅੰਤਰਣ ਦੀ ਮਿਆਦ</t>
+          <t>ਟ੍ਰਾਂਸਕ੍ਰਾਈਬ ਦੀ ਮਿਆਦ</t>
         </is>
       </c>
       <c r="L146" t="inlineStr">
@@ -9944,7 +9944,7 @@
       <c r="D149" t="inlineStr"/>
       <c r="E149" t="inlineStr">
         <is>
-          <t>ઇમેજનું લેબલિંગ કરવામાં આવ્યું</t>
+          <t>લેબલિંગ થયેલી ઇમેજ</t>
         </is>
       </c>
       <c r="F149" t="inlineStr">
@@ -9974,7 +9974,7 @@
       </c>
       <c r="K149" t="inlineStr">
         <is>
-          <t>ਲੇਬਲ ਕੀਤੀਆਂ ਗਈਆਂ ਇਮੇਜਾਂ</t>
+          <t>ਲੇਬਲ ਕੀਤੀਆਂ ਗਈਆਂ ਇਮੇਜਸ</t>
         </is>
       </c>
       <c r="L149" t="inlineStr">
@@ -10012,7 +10012,7 @@
       <c r="D150" t="inlineStr"/>
       <c r="E150" t="inlineStr">
         <is>
-          <t>ઇમેજ માન્ય કરવામાં આવી</t>
+          <t>માન્ય  ઇમેજ</t>
         </is>
       </c>
       <c r="F150" t="inlineStr">
@@ -10042,7 +10042,7 @@
       </c>
       <c r="K150" t="inlineStr">
         <is>
-          <t>ਪ੍ਰਮਾਣਿਤ ਕੀਤੀਆਂ ਗਈਆਂ ਇਮੇਜਾਂ</t>
+          <t>ਪ੍ਰਮਾਣਿਤ ਇਮੇਜਸ</t>
         </is>
       </c>
       <c r="L150" t="inlineStr">
@@ -10178,7 +10178,7 @@
       </c>
       <c r="K152" t="inlineStr">
         <is>
-          <t>ਅਨੁਵਾਦਾਂ ਨੂੰ ਪ੍ਰਮਾਣਿਤ ਕੀਤਾ ਗਿਆ</t>
+          <t>ਪ੍ਰਮਾਣਿਤ ਅਨੁਵਾਦ</t>
         </is>
       </c>
       <c r="L152" t="inlineStr">
@@ -10289,7 +10289,7 @@
       </c>
       <c r="F154" t="inlineStr">
         <is>
-          <t>Contribution Tracker</t>
+          <t>অৰিহনা ট্ৰেকাৰ</t>
         </is>
       </c>
       <c r="G154" t="inlineStr">
@@ -10357,7 +10357,7 @@
       </c>
       <c r="F155" t="inlineStr">
         <is>
-          <t>Your language and top 3 contributed languages</t>
+          <t>আপোনাৰ ভাষা আৰু শীৰ্ষ 3 টা অৱদানযুক্ত ভাষা</t>
         </is>
       </c>
       <c r="G155" t="inlineStr">
@@ -10382,7 +10382,7 @@
       </c>
       <c r="K155" t="inlineStr">
         <is>
-          <t>ਤੁਹਾਡੀ ਭਾਸ਼ਾ ਅਤੇ ਚੋਟੀ ਦੀਆਂ 3 ਯੋਗਦਾਨ ਪਾਉਣ ਵਾਲੀਆਂ ਭਾਸ਼ਾਵਾਂ</t>
+          <t>ਤੁਹਾਡੀ ਭਾਸ਼ਾ ਅਤੇ ਸਿਖਰਲੀਆਂ 3 ਯੋਗਦਾਨ ਪਾਉਣ ਵਾਲੀਆਂ ਭਾਸ਼ਾਵਾਂ</t>
         </is>
       </c>
       <c r="L155" t="inlineStr">
@@ -10425,7 +10425,7 @@
       </c>
       <c r="F156" t="inlineStr">
         <is>
-          <t>আপোনাৰ ভাষা যোৰ আৰু শীৰ্ষ ৩ টা সৰ্বাধিক অৱদান প্ৰাপ্ত ভাষাৰ যোৰ</t>
+          <t>আপোনাৰ ভাষাৰ যোৰ আৰু শীৰ্ষ 3 টা অৱদান আগবঢ়োৱা ভাষাৰ</t>
         </is>
       </c>
       <c r="G156" t="inlineStr">
@@ -10488,12 +10488,12 @@
       <c r="D157" t="inlineStr"/>
       <c r="E157" t="inlineStr">
         <is>
-          <t>કલાક</t>
+          <t>કલાક ના આધારે</t>
         </is>
       </c>
       <c r="F157" t="inlineStr">
         <is>
-          <t>By duration of hours</t>
+          <t>ঘন্টাৰ কালদৈৰ্ঘ্যৰ দ্বাৰা</t>
         </is>
       </c>
       <c r="G157" t="inlineStr">
@@ -10561,7 +10561,7 @@
       </c>
       <c r="F158" t="inlineStr">
         <is>
-          <t>By number of sentences</t>
+          <t>বাক্যৰ সংখ্যাৰ দ্বাৰা</t>
         </is>
       </c>
       <c r="G158" t="inlineStr">
@@ -10697,7 +10697,7 @@
       </c>
       <c r="F160" t="inlineStr">
         <is>
-          <t>Total sentences</t>
+          <t>মুঠ বাক্য</t>
         </is>
       </c>
       <c r="G160" t="inlineStr">
@@ -10765,7 +10765,7 @@
       </c>
       <c r="F161" t="inlineStr">
         <is>
-          <t>Total recordings</t>
+          <t>মুুঠ ৰেকৰ্ডিং</t>
         </is>
       </c>
       <c r="G161" t="inlineStr">
@@ -10911,7 +10911,7 @@
       </c>
       <c r="H163" t="inlineStr">
         <is>
-          <t>சரிபார்க்கப்பட்ட மற்றும் லேபிள் செய்யப்பட்ட  படங்கள்</t>
+          <t>சரிபார்க்கப்பட்ட மற்றும் லேபிள் செய்யப்பட்ட படங்கள்</t>
         </is>
       </c>
       <c r="I163" t="inlineStr">
@@ -11037,7 +11037,7 @@
       </c>
       <c r="F165" t="inlineStr">
         <is>
-          <t>Speakers</t>
+          <t>বক্তা</t>
         </is>
       </c>
       <c r="G165" t="inlineStr">
@@ -11062,7 +11062,7 @@
       </c>
       <c r="K165" t="inlineStr">
         <is>
-          <t>ਸਪੀਕਰ</t>
+          <t>ਵਕਤਾ</t>
         </is>
       </c>
       <c r="L165" t="inlineStr">
@@ -11105,7 +11105,7 @@
       </c>
       <c r="F166" t="inlineStr">
         <is>
-          <t>Translations</t>
+          <t>অনুবাদ</t>
         </is>
       </c>
       <c r="G166" t="inlineStr">
@@ -11638,7 +11638,7 @@
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>ट्रांसक्राइब  करें</t>
+          <t>ट्रांसक्राइब करें</t>
         </is>
       </c>
       <c r="D174" t="inlineStr"/>
@@ -11659,7 +11659,7 @@
       </c>
       <c r="H174" t="inlineStr">
         <is>
-          <t>எடுத்தெழுது</t>
+          <t>டிரான்ஸ்க்ரைப் செய்</t>
         </is>
       </c>
       <c r="I174" t="inlineStr">
@@ -11674,7 +11674,7 @@
       </c>
       <c r="K174" t="inlineStr">
         <is>
-          <t>ਲਿਪੀਅੰਤਰਣ ਕਰੋ</t>
+          <t>ਟ੍ਰਾਂਸਕ੍ਰਾਈਬ ਕਰੋ</t>
         </is>
       </c>
       <c r="L174" t="inlineStr">
@@ -11785,7 +11785,7 @@
       </c>
       <c r="F176" t="inlineStr">
         <is>
-          <t>Contribute</t>
+          <t>অৰিহণা</t>
         </is>
       </c>
       <c r="G176" t="inlineStr">
@@ -14034,7 +14034,7 @@
       </c>
       <c r="G209" t="inlineStr">
         <is>
-          <t>ঘৃণ্য / বৈষম্যমূলক / অশ্লীল ভাষা, মাদকের প্রচার ইত্যাদি</t>
+          <t>ঘৃণ্য / বৈষম্যমূলক / অশ্লীল ভাষা, মাদকের প্রচার ইত্যাদি।</t>
         </is>
       </c>
       <c r="H209" t="inlineStr">
@@ -14054,7 +14054,7 @@
       </c>
       <c r="K209" t="inlineStr">
         <is>
-          <t>ਨਫ਼ਰਤ ਭਰੀ / ਵਿਤਕਰੇ ਵਾਲੀ / ਅਸ਼ਲੀਲ ਭਾਸ਼ਾ, ਨਸ਼ਿਆਂ ਨੂੰ ਉਤਸ਼ਾਹਿਤ ਕਰਨਾ ਆਦਿ</t>
+          <t>ਨਫ਼ਰਤ ਫੈਲਾਉਣ ਵਾਲੀ / ਭੇਦਭਾਵ ਵਾਲੀ / ਅਸ਼ਲੀਲ ਭਾਸ਼ਾ, ਨਸ਼ੀਲੀਆਂ ਦਵਾਈਆਂ ਦਾ ਪ੍ਰਚਾਰ ਆਦਿ</t>
         </is>
       </c>
       <c r="L209" t="inlineStr">
@@ -14154,7 +14154,7 @@
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>धन्यवाद!</t>
+          <t>धन्यवाद</t>
         </is>
       </c>
       <c r="D211" t="inlineStr"/>
@@ -14530,7 +14530,7 @@
       </c>
       <c r="K216" t="inlineStr">
         <is>
-          <t>ਸਕਿਪ</t>
+          <t>ਸਕਿਪ ਕਰੋ</t>
         </is>
       </c>
       <c r="L216" t="inlineStr">
@@ -14666,7 +14666,7 @@
       </c>
       <c r="K218" t="inlineStr">
         <is>
-          <t>ਸੁਧਾਰ ਕਰਨ ਲਈ ਤੁਹਾਡਾ ਸ਼ੁਕਰੀਆ!</t>
+          <t>ਸੁਧਾਰਨ ਦੇ ਲਈ ਤੁਹਾਡਾ ਸ਼ੁਕਰੀਆ!</t>
         </is>
       </c>
       <c r="L218" t="inlineStr">
@@ -14734,7 +14734,7 @@
       </c>
       <c r="K219" t="inlineStr">
         <is>
-          <t>ਆਪਣੀ ਆਵਾਜ਼ ਦਾ ਯੋਗਦਾਨ ਪਾਉਣ ਲਈ ਤੁਹਾਡੇ ਵੱਲੋਂ ਦਿਖਾਏ ਗਏ ਉਤਸ਼ਾਹ ਲਈ ਸ਼ੁਕਰੀਆ।</t>
+          <t>ਆਪਣੀ ਆਵਾਜ਼ ਦਾ ਯੋਗਦਾਨ ਪਾਉਣ ਲਈ ਦਿਖਾਏ ਗਏ ਉਤਸ਼ਾਹ ਲਈ ਤੁਹਾਡਾ ਸ਼ੁਕਰੀਆ।</t>
         </is>
       </c>
       <c r="L219" t="inlineStr">
@@ -14766,7 +14766,7 @@
       </c>
       <c r="C220" t="inlineStr">
         <is>
-          <t>पूरे उत्साह के साथ रिकॉर्डिंग को ट्रांसक्राइब करने के लिए धन्यवाद!</t>
+          <t>पूरे उत्साह के साथ रिकॉर्डिंग को ट्रांसक्राइब करने के लिए धन्यवाद</t>
         </is>
       </c>
       <c r="D220" t="inlineStr"/>
@@ -14802,7 +14802,7 @@
       </c>
       <c r="K220" t="inlineStr">
         <is>
-          <t>ਪੂਰੇ ਉਤਸ਼ਾਹ ਨਾਲ ਰਿਕਾਰਡਿੰਗ ਨੂੰ ਲਿਪੀਅੰਤ੍ਰਿਤ ਕਰਨ ਲਈ ਤੁਹਾਡਾ ਸ਼ੁਕਰੀਆ।</t>
+          <t>ਪੂਰੇ ਉਤਸ਼ਾਹ ਨਾਲ ਰਿਕਾਰਡਿੰਗ ਨੂੰ ਟ੍ਰਾਂਸਕ੍ਰਾਈਬ ਕਰਨ ਲਈ ਤੁਹਾਡਾ ਸ਼ੁਕਰੀਆ।</t>
         </is>
       </c>
       <c r="L220" t="inlineStr">
@@ -14902,7 +14902,7 @@
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>पूरे उत्साह के साथ इमेज को लेबल करने के लिए धन्यवाद!</t>
+          <t>पूरे उत्साह के साथ इमेज को लेबल करने के लिए धन्यवाद</t>
         </is>
       </c>
       <c r="D222" t="inlineStr"/>
@@ -14970,7 +14970,7 @@
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>पूरे उत्साह के साथ रिकॉर्डिंग्स को सत्यापित करने के लिए धन्यवाद!</t>
+          <t>पूरे उत्साह के साथ रिकॉर्डिंग्स को सत्यापित करने के लिए धन्यवाद</t>
         </is>
       </c>
       <c r="D223" t="inlineStr"/>
@@ -15278,7 +15278,7 @@
       </c>
       <c r="K227" t="inlineStr">
         <is>
-          <t>ਕੈਂਸਲ</t>
+          <t>ਕੈਂਸਲ ਕਰੋ</t>
         </is>
       </c>
       <c r="L227" t="inlineStr">
@@ -15482,7 +15482,7 @@
       </c>
       <c r="K230" t="inlineStr">
         <is>
-          <t>ਰੀ-ਪਲੇਅ</t>
+          <t>ਰੀ-ਪਲੇਅ ਕਰੋ</t>
         </is>
       </c>
       <c r="L230" t="inlineStr">
@@ -15514,7 +15514,7 @@
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>रिपोर्ट  करें</t>
+          <t>रिपोर्ट करें</t>
         </is>
       </c>
       <c r="D231" t="inlineStr"/>
@@ -15603,7 +15603,7 @@
       </c>
       <c r="H232" t="inlineStr">
         <is>
-          <t>உங்கள் ஒலிபெருக்கிச் சோதிக்கவும்</t>
+          <t>உங்கள் ஒலிபெருக்கியைச் சோதிக்கவும்</t>
         </is>
       </c>
       <c r="I232" t="inlineStr">
@@ -16298,7 +16298,7 @@
       </c>
       <c r="K242" t="inlineStr">
         <is>
-          <t>ਟੈਕਸਟ ਜੋੜੋ</t>
+          <t>ਟੈਕਸਟ ਲਿਖੋ</t>
         </is>
       </c>
       <c r="L242" t="inlineStr">
@@ -16570,7 +16570,7 @@
       </c>
       <c r="K246" t="inlineStr">
         <is>
-          <t>ਵਿਸ਼ੇਸ਼ ਅੱਖਰਾਂ ਦੀ ਵਰਤੋਂ ਦੀ ਇਜਾਜ਼ਤ ਨਹੀਂ ਹੈ</t>
+          <t>ਵਿਸ਼ੇਸ਼ ਅੱਖਰਾਂ ਦੀ ਵਰਤੋਂ ਸੰਭਵ ਨਹੀਂ</t>
         </is>
       </c>
       <c r="L246" t="inlineStr">
@@ -16874,7 +16874,7 @@
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>किसी एक भाषा को चुनें</t>
+          <t>भाषा चुनें</t>
         </is>
       </c>
       <c r="D251" t="inlineStr"/>
@@ -16910,7 +16910,7 @@
       </c>
       <c r="K251" t="inlineStr">
         <is>
-          <t>ਕੋਈ ਇੱਕ ਭਾਸ਼ਾ ਚੁਣੋ</t>
+          <t>ਭਾਸ਼ਾ ਚੁਣੋ</t>
         </is>
       </c>
       <c r="L251" t="inlineStr">
@@ -17046,7 +17046,7 @@
       </c>
       <c r="K253" t="inlineStr">
         <is>
-          <t>ਪਿਛਲਾ ਅਪਡੇਟ ਕੀਤਾ ਡਾਟਾ</t>
+          <t>ਪਿਛਲਾ ਡਾਟਾ ਅਪਡੇਟ</t>
         </is>
       </c>
       <c r="L253" t="inlineStr">
@@ -17157,7 +17157,7 @@
       </c>
       <c r="F255" t="inlineStr">
         <is>
-          <t>People</t>
+          <t>ব্যক্তি</t>
         </is>
       </c>
       <c r="G255" t="inlineStr">
@@ -17225,7 +17225,7 @@
       </c>
       <c r="F256" t="inlineStr">
         <is>
-          <t>Transcribed</t>
+          <t>প্ৰতিলিপিকৃত</t>
         </is>
       </c>
       <c r="G256" t="inlineStr">
@@ -17235,7 +17235,7 @@
       </c>
       <c r="H256" t="inlineStr">
         <is>
-          <t>எடுத்தெழுதப்பட்டது</t>
+          <t>டிரான்ஸ்க்ரைப்டு</t>
         </is>
       </c>
       <c r="I256" t="inlineStr">
@@ -17250,7 +17250,7 @@
       </c>
       <c r="K256" t="inlineStr">
         <is>
-          <t>ਲਿਪੀਅੰਤਰਣ</t>
+          <t>ਟ੍ਰਾਂਸਕ੍ਰਾਈਬਡ</t>
         </is>
       </c>
       <c r="L256" t="inlineStr">
@@ -17293,7 +17293,7 @@
       </c>
       <c r="F257" t="inlineStr">
         <is>
-          <t>Contributed</t>
+          <t>অৱদান আগবঢ়োৱা</t>
         </is>
       </c>
       <c r="G257" t="inlineStr">
@@ -17361,7 +17361,7 @@
       </c>
       <c r="F258" t="inlineStr">
         <is>
-          <t>Labelled</t>
+          <t>লেবেল প্ৰদান কৰা</t>
         </is>
       </c>
       <c r="G258" t="inlineStr">
@@ -17429,7 +17429,7 @@
       </c>
       <c r="F259" t="inlineStr">
         <is>
-          <t>Translated</t>
+          <t>অনুবাদিত</t>
         </is>
       </c>
       <c r="G259" t="inlineStr">
@@ -17492,12 +17492,12 @@
       <c r="D260" t="inlineStr"/>
       <c r="E260" t="inlineStr">
         <is>
-          <t>ચકાસો</t>
+          <t>માન્ય</t>
         </is>
       </c>
       <c r="F260" t="inlineStr">
         <is>
-          <t>Validated</t>
+          <t>বৈধতা প্ৰদান কৰা</t>
         </is>
       </c>
       <c r="G260" t="inlineStr">
@@ -17590,7 +17590,7 @@
       </c>
       <c r="K261" t="inlineStr">
         <is>
-          <t>ਰਾਜ ਅਨੁਸਾਰ ਵੇਰਵਾ</t>
+          <t>ਰਾਜ ਅਨੁਸਾਰ ਵੰਡ</t>
         </is>
       </c>
       <c r="L261" t="inlineStr">
@@ -17726,7 +17726,7 @@
       </c>
       <c r="K263" t="inlineStr">
         <is>
-          <t>ਲਿੰਗਿਕ ਵਰਗੀਕਰਨ</t>
+          <t>ਲਿੰਗਿਕ ਵੇਰਵਾ</t>
         </is>
       </c>
       <c r="L263" t="inlineStr">
@@ -17794,7 +17794,7 @@
       </c>
       <c r="K264" t="inlineStr">
         <is>
-          <t>ਉਮਰ ਵਰਗ ਦਾ ਵੇਰਵਾ</t>
+          <t>ਉਮਰ ਵਰਗ ਦੀ ਵੰਡ</t>
         </is>
       </c>
       <c r="L264" t="inlineStr">
@@ -17862,7 +17862,7 @@
       </c>
       <c r="K265" t="inlineStr">
         <is>
-          <t>ਸਹੀ</t>
+          <t>ਸਹੀ ਹੈ</t>
         </is>
       </c>
       <c r="L265" t="inlineStr">
@@ -17920,7 +17920,7 @@
       </c>
       <c r="I266" t="inlineStr">
         <is>
-          <t>మార్చాలి</t>
+          <t>మార్చాల్సిన అవసరం ఉంది</t>
         </is>
       </c>
       <c r="J266" t="inlineStr">
@@ -18177,7 +18177,7 @@
       </c>
       <c r="F270" t="inlineStr">
         <is>
-          <t>Congratulations on winning a new badge!</t>
+          <t>এটা নতুন বেজ জয় কৰাৰ বাবে অভিনন্দন!</t>
         </is>
       </c>
       <c r="G270" t="inlineStr">
@@ -18245,12 +18245,12 @@
       </c>
       <c r="F271" t="inlineStr">
         <is>
-          <t>Contribute to your language!</t>
+          <t>আপোনাৰ ভাষালৈ অৱদান আগবঢ়াওক৷</t>
         </is>
       </c>
       <c r="G271" t="inlineStr">
         <is>
-          <t>আপনার ভাষার জন্য যোগদান দিন !</t>
+          <t>আপনার ভাষার জন্য যোগদান দিন!</t>
         </is>
       </c>
       <c r="H271" t="inlineStr">
@@ -18454,7 +18454,7 @@
       </c>
       <c r="G274" t="inlineStr">
         <is>
-          <t>বন্ধ করুন</t>
+          <t>এখন যোগদান দিন</t>
         </is>
       </c>
       <c r="H274" t="inlineStr">
@@ -18517,7 +18517,7 @@
       </c>
       <c r="F275" t="inlineStr">
         <is>
-          <t>Telangana</t>
+          <t>তেলেংগনা</t>
         </is>
       </c>
       <c r="G275" t="inlineStr">
@@ -18542,7 +18542,7 @@
       </c>
       <c r="K275" t="inlineStr">
         <is>
-          <t>ਤੇਲੰਗਾਨਾ</t>
+          <t>ਤੇਲੰਗਨਾ</t>
         </is>
       </c>
       <c r="L275" t="inlineStr">
@@ -18585,7 +18585,7 @@
       </c>
       <c r="F276" t="inlineStr">
         <is>
-          <t>Andaman and Nicobar Islands</t>
+          <t>আন্দামান আৰু নিকোবৰ দ্বীপপুঞ্জ</t>
         </is>
       </c>
       <c r="G276" t="inlineStr">
@@ -18653,7 +18653,7 @@
       </c>
       <c r="F277" t="inlineStr">
         <is>
-          <t>Andhra Pradesh</t>
+          <t>অন্ধ্ৰ প্ৰদেশ</t>
         </is>
       </c>
       <c r="G277" t="inlineStr">
@@ -18721,7 +18721,7 @@
       </c>
       <c r="F278" t="inlineStr">
         <is>
-          <t>Arunachal Pradesh</t>
+          <t>অৰুণাচল প্ৰদেশ</t>
         </is>
       </c>
       <c r="G278" t="inlineStr">
@@ -18789,7 +18789,7 @@
       </c>
       <c r="F279" t="inlineStr">
         <is>
-          <t>Assam</t>
+          <t>অসম</t>
         </is>
       </c>
       <c r="G279" t="inlineStr">
@@ -18857,7 +18857,7 @@
       </c>
       <c r="F280" t="inlineStr">
         <is>
-          <t>Bihar</t>
+          <t>বিহাৰ</t>
         </is>
       </c>
       <c r="G280" t="inlineStr">
@@ -18925,7 +18925,7 @@
       </c>
       <c r="F281" t="inlineStr">
         <is>
-          <t>Chhattisgarh</t>
+          <t>চত্তীছগড়</t>
         </is>
       </c>
       <c r="G281" t="inlineStr">
@@ -18940,7 +18940,7 @@
       </c>
       <c r="I281" t="inlineStr">
         <is>
-          <t>ఛత్తీస్‌గర్</t>
+          <t>ఛత్తీస్‌ఘర్</t>
         </is>
       </c>
       <c r="J281" t="inlineStr">
@@ -18993,7 +18993,7 @@
       </c>
       <c r="F282" t="inlineStr">
         <is>
-          <t>Goa</t>
+          <t>গোৱা</t>
         </is>
       </c>
       <c r="G282" t="inlineStr">
@@ -19061,7 +19061,7 @@
       </c>
       <c r="F283" t="inlineStr">
         <is>
-          <t>Gujarat</t>
+          <t>গুজৰাট</t>
         </is>
       </c>
       <c r="G283" t="inlineStr">
@@ -19129,7 +19129,7 @@
       </c>
       <c r="F284" t="inlineStr">
         <is>
-          <t>Haryana</t>
+          <t>হাৰিয়ানা</t>
         </is>
       </c>
       <c r="G284" t="inlineStr">
@@ -19197,7 +19197,7 @@
       </c>
       <c r="F285" t="inlineStr">
         <is>
-          <t>Himachal Pradesh</t>
+          <t>হিমাচল প্ৰদেশ</t>
         </is>
       </c>
       <c r="G285" t="inlineStr">
@@ -19265,7 +19265,7 @@
       </c>
       <c r="F286" t="inlineStr">
         <is>
-          <t>Jammu &amp; Kashmir</t>
+          <t>জম্মু- কাশ্মীৰ</t>
         </is>
       </c>
       <c r="G286" t="inlineStr">
@@ -19333,7 +19333,7 @@
       </c>
       <c r="F287" t="inlineStr">
         <is>
-          <t>Jharkhand</t>
+          <t>ঝাৰখণ্ড</t>
         </is>
       </c>
       <c r="G287" t="inlineStr">
@@ -19401,7 +19401,7 @@
       </c>
       <c r="F288" t="inlineStr">
         <is>
-          <t>Karnataka</t>
+          <t>কৰ্ণাটক</t>
         </is>
       </c>
       <c r="G288" t="inlineStr">
@@ -19469,7 +19469,7 @@
       </c>
       <c r="F289" t="inlineStr">
         <is>
-          <t>Kerala</t>
+          <t>কেৰেলা</t>
         </is>
       </c>
       <c r="G289" t="inlineStr">
@@ -19537,7 +19537,7 @@
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>Lakshadweep</t>
+          <t>লক্ষদ্বীপ</t>
         </is>
       </c>
       <c r="G290" t="inlineStr">
@@ -19605,7 +19605,7 @@
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>Madhya Pradesh</t>
+          <t>মধ্য প্ৰদেশ</t>
         </is>
       </c>
       <c r="G291" t="inlineStr">
@@ -19673,7 +19673,7 @@
       </c>
       <c r="F292" t="inlineStr">
         <is>
-          <t>Maharashtra</t>
+          <t>মহাৰাষ্ট্ৰ</t>
         </is>
       </c>
       <c r="G292" t="inlineStr">
@@ -19741,7 +19741,7 @@
       </c>
       <c r="F293" t="inlineStr">
         <is>
-          <t>Manipur</t>
+          <t>মণিপুৰ</t>
         </is>
       </c>
       <c r="G293" t="inlineStr">
@@ -19809,7 +19809,7 @@
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>Chandigarh</t>
+          <t>চণ্ডীগড়</t>
         </is>
       </c>
       <c r="G294" t="inlineStr">
@@ -19877,7 +19877,7 @@
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>Puducherry</t>
+          <t>পণ্ডিচেৰী</t>
         </is>
       </c>
       <c r="G295" t="inlineStr">
@@ -19945,7 +19945,7 @@
       </c>
       <c r="F296" t="inlineStr">
         <is>
-          <t>Punjab</t>
+          <t>পাঞ্জাৱ</t>
         </is>
       </c>
       <c r="G296" t="inlineStr">
@@ -20013,7 +20013,7 @@
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>Rajasthan</t>
+          <t>ৰাজস্থান</t>
         </is>
       </c>
       <c r="G297" t="inlineStr">
@@ -20081,7 +20081,7 @@
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>Sikkim</t>
+          <t>চিক্কিম</t>
         </is>
       </c>
       <c r="G298" t="inlineStr">
@@ -20149,7 +20149,7 @@
       </c>
       <c r="F299" t="inlineStr">
         <is>
-          <t>Tamil Nadu</t>
+          <t>তামিলনাডু</t>
         </is>
       </c>
       <c r="G299" t="inlineStr">
@@ -20217,7 +20217,7 @@
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>Tripura</t>
+          <t>ত্ৰিপুৰা</t>
         </is>
       </c>
       <c r="G300" t="inlineStr">
@@ -20285,7 +20285,7 @@
       </c>
       <c r="F301" t="inlineStr">
         <is>
-          <t>Uttar Pradesh</t>
+          <t>উত্তৰ প্ৰদেশ</t>
         </is>
       </c>
       <c r="G301" t="inlineStr">
@@ -20353,7 +20353,7 @@
       </c>
       <c r="F302" t="inlineStr">
         <is>
-          <t>Uttarakhand</t>
+          <t>উত্তৰাখণ্ড</t>
         </is>
       </c>
       <c r="G302" t="inlineStr">
@@ -20421,7 +20421,7 @@
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>West Bengal</t>
+          <t>পশ্চিম বংগ</t>
         </is>
       </c>
       <c r="G303" t="inlineStr">
@@ -20489,7 +20489,7 @@
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>Odisha</t>
+          <t>উড়িষ্যা</t>
         </is>
       </c>
       <c r="G304" t="inlineStr">
@@ -20514,7 +20514,7 @@
       </c>
       <c r="K304" t="inlineStr">
         <is>
-          <t>ਉੜੀਸਾ</t>
+          <t>ਓਡਿਸ਼ਾ</t>
         </is>
       </c>
       <c r="L304" t="inlineStr">
@@ -20557,7 +20557,7 @@
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>Dadra and Nagar Haveli and Daman and Diu</t>
+          <t>দাদৰা আৰু নগৰ হাভেলী আৰু দমন-দিউ</t>
         </is>
       </c>
       <c r="G305" t="inlineStr">
@@ -20625,7 +20625,7 @@
       </c>
       <c r="F306" t="inlineStr">
         <is>
-          <t>Meghalaya</t>
+          <t>মেঘালয়</t>
         </is>
       </c>
       <c r="G306" t="inlineStr">
@@ -20693,7 +20693,7 @@
       </c>
       <c r="F307" t="inlineStr">
         <is>
-          <t>Mizoram</t>
+          <t>মিজোৰাম</t>
         </is>
       </c>
       <c r="G307" t="inlineStr">
@@ -20761,7 +20761,7 @@
       </c>
       <c r="F308" t="inlineStr">
         <is>
-          <t>Nagaland</t>
+          <t>নাগালেণ্ড</t>
         </is>
       </c>
       <c r="G308" t="inlineStr">
@@ -20829,7 +20829,7 @@
       </c>
       <c r="F309" t="inlineStr">
         <is>
-          <t>National Capital Territory of Delhi</t>
+          <t>ৰাষ্ট্ৰৰ ৰাজধানী দিল্লীৰ ভূখণ্ড</t>
         </is>
       </c>
       <c r="G309" t="inlineStr">
@@ -20897,7 +20897,7 @@
       </c>
       <c r="F310" t="inlineStr">
         <is>
-          <t>Ladakh</t>
+          <t>লাদাখ</t>
         </is>
       </c>
       <c r="G310" t="inlineStr">
@@ -20965,7 +20965,7 @@
       </c>
       <c r="F311" t="inlineStr">
         <is>
-          <t>Your Badges</t>
+          <t>আপোনাৰ বেজ সমূহ</t>
         </is>
       </c>
       <c r="G311" t="inlineStr">
@@ -21033,7 +21033,7 @@
       </c>
       <c r="F312" t="inlineStr">
         <is>
-          <t>&lt;ভাষা&gt;ক শীৰ্ষ 3 ত চাবলৈ অংশগ্ৰহণ কৰক</t>
+          <t>{{language}}ক শীৰ্ষ 3 ত চাবলৈ অংশগ্ৰহণ কৰক</t>
         </is>
       </c>
       <c r="G312" t="inlineStr">
@@ -21101,7 +21101,7 @@
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>&lt;ভাষা&gt;ক শীৰ্ষ 3 ত ত ৰাখিবলৈ অংশগ্ৰহণ কৰক</t>
+          <t>{{language}}ক শীৰ্ষ 3 ত ত ৰাখিবলৈ অংশগ্ৰহণ কৰক</t>
         </is>
       </c>
       <c r="G313" t="inlineStr">
@@ -21294,58 +21294,58 @@
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>Contribute to see your language on top</t>
+          <t>अपनी भाषा को शीर्ष पर देखने के लिए योगदान दें</t>
         </is>
       </c>
       <c r="D316" t="inlineStr"/>
       <c r="E316" t="inlineStr">
         <is>
+          <t>તમારી ભાષાને ટોચ પર જોવા માટે યોગદાન આપો</t>
+        </is>
+      </c>
+      <c r="F316" t="inlineStr">
+        <is>
           <t>Contribute to see your language on top</t>
         </is>
       </c>
-      <c r="F316" t="inlineStr">
-        <is>
-          <t>Contribute to see your language on top</t>
-        </is>
-      </c>
       <c r="G316" t="inlineStr">
         <is>
-          <t>Contribute to see your language on top</t>
+          <t>আপনার ভাষাকে শীর্ষে দেখতে যোগদান দিন</t>
         </is>
       </c>
       <c r="H316" t="inlineStr">
         <is>
-          <t>Contribute to see your language on top</t>
+          <t>உங்கள் மொழியை முதலிடத்தில் காண பங்களிக்கவும்</t>
         </is>
       </c>
       <c r="I316" t="inlineStr">
         <is>
-          <t>Contribute to see your language on top</t>
+          <t>అగ్రస్ధానంలో మీ భాషను చూసేందుకు కాంట్రిబ్యూట్ చేయండి</t>
         </is>
       </c>
       <c r="J316" t="inlineStr">
         <is>
-          <t>Contribute to see your language on top</t>
+          <t>आपल्या भाषेला सर्वोच्च स्थानी ठेवण्यासाठी योगदान करा</t>
         </is>
       </c>
       <c r="K316" t="inlineStr">
         <is>
-          <t>Contribute to see your language on top</t>
+          <t>ਆਪਣੀ ਭਾਸ਼ਾ ਨੂੰ ਸਿਖਰ 'ਤੇ ਦੇਖਣ ਲਈ ਯੋਗਦਾਨ ਪਾਓ</t>
         </is>
       </c>
       <c r="L316" t="inlineStr">
         <is>
-          <t>Contribute to see your language on top</t>
+          <t>നിങ്ങളുടെ ഭാഷയെ ഒന്നാമത് കാണുന്നതിനായി സംഭാവന ചെയ്യുക</t>
         </is>
       </c>
       <c r="M316" t="inlineStr">
         <is>
-          <t>Contribute to see your language on top</t>
+          <t>ନିଜ ଭାଷାକୁ ଶୀର୍ଷରେ ଦେଖିବା ପାଇଁ ଯୋଗଦାନ କରନ୍ତୁ</t>
         </is>
       </c>
       <c r="N316" t="inlineStr">
         <is>
-          <t>Contribute to see your language on top</t>
+          <t>ನಿಮ್ಮ ಭಾಷೆಯನ್ನು ಅಘ್ರ ಸ್ಥಾನದಲ್ಲಿಡಲು ಕೊಡುಗೆ ನೀಡಿ</t>
         </is>
       </c>
     </row>
@@ -21362,58 +21362,58 @@
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>Validate to see your language on top</t>
+          <t>अपनी भाषा को शीर्ष पर देखने के लिए पुष्टि करें</t>
         </is>
       </c>
       <c r="D317" t="inlineStr"/>
       <c r="E317" t="inlineStr">
         <is>
+          <t>તમારી ભાષાને ટોચ પર જોવા  માટે માન્ય કરો</t>
+        </is>
+      </c>
+      <c r="F317" t="inlineStr">
+        <is>
           <t>Validate to see your language on top</t>
         </is>
       </c>
-      <c r="F317" t="inlineStr">
-        <is>
-          <t>Validate to see your language on top</t>
-        </is>
-      </c>
       <c r="G317" t="inlineStr">
         <is>
-          <t>Validate to see your language on top</t>
+          <t>আপনার ভাষাকে শীর্ষে দেখতে যাচাই করুন</t>
         </is>
       </c>
       <c r="H317" t="inlineStr">
         <is>
-          <t>Validate to see your language on top</t>
+          <t>உங்கள் மொழியை முதலிடத்தில் பார்க்க சரிபார்க்கவும்</t>
         </is>
       </c>
       <c r="I317" t="inlineStr">
         <is>
-          <t>Validate to see your language on top</t>
+          <t>అగ్రస్ధానంలో మీ భాషను చూసేందుకు ధృవీకరించండి</t>
         </is>
       </c>
       <c r="J317" t="inlineStr">
         <is>
-          <t>Validate to see your language on top</t>
+          <t>आपल्या भाषेला सर्वोच्च स्थानी ठेवण्यासाठी मूल्यांकन करा</t>
         </is>
       </c>
       <c r="K317" t="inlineStr">
         <is>
-          <t>Validate to see your language on top</t>
+          <t>ਆਪਣੀ ਭਾਸ਼ਾ ਨੂੰ ਸਿਖਰ 'ਤੇ ਦੇਖਣ ਲਈ ਪ੍ਰਮਾਣਿਤ ਕਰੋ</t>
         </is>
       </c>
       <c r="L317" t="inlineStr">
         <is>
-          <t>Validate to see your language on top</t>
+          <t>നിങ്ങളുടെ ഭാഷയെ ഒന്നാമത് കാണുന്നതിനായി സാധൂകരിക്കുക</t>
         </is>
       </c>
       <c r="M317" t="inlineStr">
         <is>
-          <t>Validate to see your language on top</t>
+          <t>ନିଜ ଭାଷାକୁ ଶୀର୍ଷରେ ଦେଖିବା ପାଇଁ ପ୍ରାମାଣିକତା ସାବ୍ୟସ୍ତ କରନ୍ତୁ</t>
         </is>
       </c>
       <c r="N317" t="inlineStr">
         <is>
-          <t>Validate to see your language on top</t>
+          <t>ನಿಮ್ಮ ಭಾಷೆಯನ್ನು ಅಘ್ರ ಸ್ಥಾನದಲ್ಲಿಡಲು ಪರಿಶೀಲನೆ ಮಾಡಿ</t>
         </is>
       </c>
     </row>
@@ -21430,58 +21430,58 @@
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>Contribute to keep your language on top</t>
+          <t>अपनी भाषा को शीर्ष पर रखने में योगदान दें</t>
         </is>
       </c>
       <c r="D318" t="inlineStr"/>
       <c r="E318" t="inlineStr">
         <is>
+          <t>તમારી ભાષાને ટોચ પર રાખવા માટે યોગદાન આપો</t>
+        </is>
+      </c>
+      <c r="F318" t="inlineStr">
+        <is>
           <t>Contribute to keep your language on top</t>
         </is>
       </c>
-      <c r="F318" t="inlineStr">
-        <is>
-          <t>Contribute to keep your language on top</t>
-        </is>
-      </c>
       <c r="G318" t="inlineStr">
         <is>
-          <t>Contribute to keep your language on top</t>
+          <t>আপনার ভাষাকে শীর্ষে রাখতে যোগদান দিন</t>
         </is>
       </c>
       <c r="H318" t="inlineStr">
         <is>
-          <t>Contribute to keep your language on top</t>
+          <t>உங்கள் மொழியை முதலிடத்தில் வைத்திருக்க பங்களிக்கவும்</t>
         </is>
       </c>
       <c r="I318" t="inlineStr">
         <is>
-          <t>Contribute to keep your language on top</t>
+          <t>మీ భాషను అగ్రస్థానంలో ఉంచడంలో సహకరించండి</t>
         </is>
       </c>
       <c r="J318" t="inlineStr">
         <is>
-          <t>Contribute to keep your language on top</t>
+          <t>आपल्या भाषेला सर्वोच्च स्थानी  ठेवण्यासाठी योगदान द्या</t>
         </is>
       </c>
       <c r="K318" t="inlineStr">
         <is>
-          <t>Contribute to keep your language on top</t>
+          <t>ਆਪਣੀ ਭਾਸ਼ਾ ਨੂੰ ਸਿਖਰ 'ਤੇ ਰੱਖਣ ਲਈ ਯੋਗਦਾਨ ਪਾਓ</t>
         </is>
       </c>
       <c r="L318" t="inlineStr">
         <is>
-          <t>Contribute to keep your language on top</t>
+          <t>നിങ്ങളുടെ ഭാഷ ഏറ്റവും മുകളില്‍ തുടരുന്നതിനായി സംഭാവന ചെയ്യുക</t>
         </is>
       </c>
       <c r="M318" t="inlineStr">
         <is>
-          <t>Contribute to keep your language on top</t>
+          <t>ନିଜ ଭାଷାକୁ ଶୀର୍ଷରେ ବଜାୟ ରଖିବା ପାଇଁ ଯୋଗଦାନ କରନ୍ତୁ</t>
         </is>
       </c>
       <c r="N318" t="inlineStr">
         <is>
-          <t>Contribute to keep your language on top</t>
+          <t>ನಿಮ್ಮ ಭಾಷೆಯನ್ನು ಅಘ್ರ ಸ್ಥಾನದಲ್ಲಿಡಲು ಕೊಡುಗೆ ನೀಡಿ</t>
         </is>
       </c>
     </row>
@@ -21498,58 +21498,58 @@
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>Validate to keep your language on top</t>
+          <t>अपनी भाषा को शीर्ष पर रखने के लिए पुष्टि करें</t>
         </is>
       </c>
       <c r="D319" t="inlineStr"/>
       <c r="E319" t="inlineStr">
         <is>
+          <t>તમારી ભાષાને ટોચ પર રાખવા માટે માન્ય કરો</t>
+        </is>
+      </c>
+      <c r="F319" t="inlineStr">
+        <is>
           <t>Validate to keep your language on top</t>
         </is>
       </c>
-      <c r="F319" t="inlineStr">
-        <is>
-          <t>Validate to keep your language on top</t>
-        </is>
-      </c>
       <c r="G319" t="inlineStr">
         <is>
-          <t>Validate to keep your language on top</t>
+          <t>আপনার ভাষাকে শীর্ষে রাখতে যাচাই করুন</t>
         </is>
       </c>
       <c r="H319" t="inlineStr">
         <is>
-          <t>Validate to keep your language on top</t>
+          <t>உங்கள் மொழியை முதலிடத்தில் வைத்திருக்க சரிபார்க்கவும்</t>
         </is>
       </c>
       <c r="I319" t="inlineStr">
         <is>
-          <t>Validate to keep your language on top</t>
+          <t>మీ భాషను అగ్రస్థానంలో ఉంచడంలో ధృవీకరించండి</t>
         </is>
       </c>
       <c r="J319" t="inlineStr">
         <is>
-          <t>Validate to keep your language on top</t>
+          <t>आपल्या भाषेला सर्वोच्च स्थानी ठेवण्यासाठी प्रमाणित करा</t>
         </is>
       </c>
       <c r="K319" t="inlineStr">
         <is>
-          <t>Validate to keep your language on top</t>
+          <t>ਆਪਣੀ ਭਾਸ਼ਾ ਨੂੰ ਸਿਖਰ 'ਤੇ ਰੱਖਣ ਲਈ ਪ੍ਰਮਾਣਿਤ ਕਰੋ</t>
         </is>
       </c>
       <c r="L319" t="inlineStr">
         <is>
-          <t>Validate to keep your language on top</t>
+          <t>നിങ്ങളുടെ ഭാഷ ഏറ്റവും മുകളില്‍ തുടരുന്നതിനായി സാധൂകരിക്കുക</t>
         </is>
       </c>
       <c r="M319" t="inlineStr">
         <is>
-          <t>Validate to keep your language on top</t>
+          <t>ନିଜ ଭାଷାକୁ ଶୀର୍ଷରେ ବଜାୟ ରଖିବା ପାଇଁ ପ୍ରାମାଣିକତା ସାବ୍ୟସ୍ତ କରନ୍ତୁ</t>
         </is>
       </c>
       <c r="N319" t="inlineStr">
         <is>
-          <t>Validate to keep your language on top</t>
+          <t>ನಿಮ್ಮ ಭಾಷೆಯನ್ನು ಅಘ್ರ ಸ್ಥಾನದಲ್ಲಿಡಲು ಪರಿಶೀಲನೆ ಮಾಡಿ</t>
         </is>
       </c>
     </row>
@@ -21645,7 +21645,7 @@
       </c>
       <c r="F321" t="inlineStr">
         <is>
-          <t>Share on</t>
+          <t>ভগাই লওক</t>
         </is>
       </c>
       <c r="G321" t="inlineStr">
@@ -21713,7 +21713,7 @@
       </c>
       <c r="F322" t="inlineStr">
         <is>
-          <t>আপুনি আপোনাৰ ভাষাৰ বাবে &lt;অৰিহণা- গণনা&gt; &lt;span&gt;বাক্যটো(বোৰ)&lt;/span&gt; অৰিহনা আগবঢ়াইছে !</t>
+          <t>আপুনি আপোনাৰ ভাষাৰ বাবে &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt;বাক্যটো(বোৰ)&lt;/span&gt; অৰিহনা আগবঢ়াইছে !</t>
         </is>
       </c>
       <c r="G322" t="inlineStr">
@@ -21781,7 +21781,7 @@
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>আপুনি আপোনাৰ ভাষাৰ বাবে &lt;অৰিহণা- গণনা&gt; &lt;span&gt;ৰেকৰ্ডিং(বোৰ)ৰ&lt;/span&gt; অৰিহনা আগবঢ়াইছে!</t>
+          <t>আপুনি আপোনাৰ ভাষাৰ বাবে &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt;ৰেকৰ্ডিং(বোৰ)ৰ&lt;/span&gt; অৰিহনা আগবঢ়াইছে!</t>
         </is>
       </c>
       <c r="G323" t="inlineStr">
@@ -21816,7 +21816,7 @@
       </c>
       <c r="M323" t="inlineStr">
         <is>
-          <t>ଆପଣ ନିଜ ଭାଷା ପାଇଁ &lt;span&gt;{{count}}&lt;/span&gt;ଟି &lt;span&gt;ରେକର୍ଡିଂର&lt;span&gt; ଯୋଗଦାନ କଲେ !</t>
+          <t>ଆପଣ ନିଜ ଭାଷା ପାଇଁ &lt;span&gt;{{count}}&lt;/span&gt;ଟି &lt;span&gt;ରେକର୍ଡିଂର&lt;/span&gt; ଯୋଗଦାନ କଲେ !</t>
         </is>
       </c>
       <c r="N323" t="inlineStr">
@@ -21849,7 +21849,7 @@
       </c>
       <c r="F324" t="inlineStr">
         <is>
-          <t>আপুনি আপোনাৰ ভাষাৰ বাবে &lt;অৰিহণা- গণনা&gt; &lt;span&gt;ছবিৰ লেবেল (সমূহ)ৰ&lt;/span&gt; অৰিহনা আগবঢ়াইছে!</t>
+          <t>আপুনি আপোনাৰ ভাষাৰ বাবে &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt;ছবিৰ লেবেল (সমূহ)ৰ&lt;/span&gt; অৰিহনা আগবঢ়াইছে!</t>
         </is>
       </c>
       <c r="G324" t="inlineStr">
@@ -21917,7 +21917,7 @@
       </c>
       <c r="F325" t="inlineStr">
         <is>
-          <t>আপুনি আপোনাৰ ভাষাৰ বাবে &lt;অৰিহণা- গণনা&gt; &lt;span&gt;বাক্যটো(বোৰ)&lt;/span&gt; অৰিহনা আগবঢ়াইছে !</t>
+          <t>আপুনি আপোনাৰ ভাষাৰ বাবে &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt;বাক্যটো(বোৰ)&lt;/span&gt; অৰিহনা আগবঢ়াইছে !</t>
         </is>
       </c>
       <c r="G325" t="inlineStr">
@@ -21985,7 +21985,7 @@
       </c>
       <c r="F326" t="inlineStr">
         <is>
-          <t>আপুনি আপোনাৰ ভাষাৰ বাবে &lt;অৰিহণা- গণনা&gt; &lt;span&gt;বাক্য (সমূহ)ৰ&lt;/span&gt; বৈধতা প্ৰদাণ কৰিছে!</t>
+          <t>আপুনি আপোনাৰ ভাষাৰ বাবে &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt;বাক্য (সমূহ)ৰ&lt;/span&gt; বৈধতা প্ৰদাণ কৰিছে!</t>
         </is>
       </c>
       <c r="G326" t="inlineStr">
@@ -22025,7 +22025,7 @@
       </c>
       <c r="N326" t="inlineStr">
         <is>
-          <t>ನಿಮ್ಮ ಭಾಷೆಗಾಗಿ ನೀವು &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt; ವಾಕ್ಯಗಳನ್ನು &lt;/&gt;  ಮೌಲ್ಯೀಕರಿಸಿದ್ದೀರಿ!</t>
+          <t>ನಿಮ್ಮ ಭಾಷೆಗಾಗಿ ನೀವು &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt; ವಾಕ್ಯಗಳನ್ನು &lt;/span&gt;  ಮೌಲ್ಯೀಕರಿಸಿದ್ದೀರಿ!</t>
         </is>
       </c>
     </row>
@@ -22053,7 +22053,7 @@
       </c>
       <c r="F327" t="inlineStr">
         <is>
-          <t>আপুনি আপোনাৰ ভাষাৰ বাবে &lt;অৰিহণা- গণনা&gt; &lt;span&gt;বাক্য (সমূহ)ৰ&lt;/span&gt; বৈধতা প্ৰদাণ কৰিছে!</t>
+          <t>আপুনি আপোনাৰ ভাষাৰ বাবে &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt;বাক্য (সমূহ)ৰ&lt;/span&gt; বৈধতা প্ৰদাণ কৰিছে!</t>
         </is>
       </c>
       <c r="G327" t="inlineStr">
@@ -22093,7 +22093,7 @@
       </c>
       <c r="N327" t="inlineStr">
         <is>
-          <t>ನಿಮ್ಮ ಭಾಷೆಗಾಗಿ ನೀವು &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt; ವಾಕ್ಯಗಳನ್ನು &lt;/&gt;  ಮೌಲ್ಯೀಕರಿಸಿದ್ದೀರಿ!</t>
+          <t>ನಿಮ್ಮ ಭಾಷೆಗಾಗಿ ನೀವು &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt; ವಾಕ್ಯಗಳನ್ನು &lt;/span&gt;  ಮೌಲ್ಯೀಕರಿಸಿದ್ದೀರಿ!</t>
         </is>
       </c>
     </row>
@@ -22121,7 +22121,7 @@
       </c>
       <c r="F328" t="inlineStr">
         <is>
-          <t>আপুনি আপোনাৰ ভাষাৰ বাবে &lt;অৰিহণা- গণনা&gt; &lt;span&gt;ছবিৰ লেবেল(বোৰ)ক&lt;/span&gt; বৈধতা প্ৰদান কৰিছে!</t>
+          <t>আপুনি আপোনাৰ ভাষাৰ বাবে &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt;ছবিৰ লেবেল(বোৰ)ক&lt;/span&gt; বৈধতা প্ৰদান কৰিছে!</t>
         </is>
       </c>
       <c r="G328" t="inlineStr">
@@ -22189,7 +22189,7 @@
       </c>
       <c r="F329" t="inlineStr">
         <is>
-          <t>আপুনি আপোনাৰ ভাষাৰ বাবে &lt;অৰিহণা- গণনা&gt; &lt;span&gt;বাক্য (সমূহ)ৰ&lt;/span&gt; বৈধতা প্ৰদাণ কৰিছে!</t>
+          <t>আপুনি আপোনাৰ ভাষাৰ বাবে &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt;বাক্য (সমূহ)ৰ&lt;/span&gt; বৈধতা প্ৰদাণ কৰিছে!</t>
         </is>
       </c>
       <c r="G329" t="inlineStr">
@@ -22229,7 +22229,7 @@
       </c>
       <c r="N329" t="inlineStr">
         <is>
-          <t>ನಿಮ್ಮ ಭಾಷೆಗಾಗಿ ನೀವು &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt; ವಾಕ್ಯಗಳನ್ನು &lt;/&gt;  ಮೌಲ್ಯೀಕರಿಸಿದ್ದೀರಿ!</t>
+          <t>ನಿಮ್ಮ ಭಾಷೆಗಾಗಿ ನೀವು &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt; ವಾಕ್ಯಗಳನ್ನು &lt;/span&gt;  ಮೌಲ್ಯೀಕರಿಸಿದ್ದೀರಿ!</t>
         </is>
       </c>
     </row>
@@ -22257,7 +22257,7 @@
       </c>
       <c r="F330" t="inlineStr">
         <is>
-          <t>আপুনি আপোনাৰ কোৱা ইণ্ডিয়া &lt;বেজ-ৰং&gt; &lt;span&gt;ভাষা সমাৰ্থক&lt;/span&gt; বেজ অৰ্জন কৰিছে৷</t>
+          <t>আপুনি আপোনাৰ কোৱা ইণ্ডিয়া &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt;ভাষা সমাৰ্থক&lt;/span&gt; বেজ অৰ্জন কৰিছে৷</t>
         </is>
       </c>
       <c r="G330" t="inlineStr">
@@ -22325,7 +22325,7 @@
       </c>
       <c r="F331" t="inlineStr">
         <is>
-          <t>আপুনি আপোনাৰ শুনা ইণ্ডিয়া &lt;বেজ-ৰং&gt; &lt;span&gt;ভাষা সমাৰ্থক&lt;/span&gt; বেজ অৰ্জন কৰিছে৷</t>
+          <t>আপুনি আপোনাৰ শুনা ইণ্ডিয়া &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt;ভাষা সমাৰ্থক&lt;/span&gt; বেজ অৰ্জন কৰিছে৷</t>
         </is>
       </c>
       <c r="G331" t="inlineStr">
@@ -22393,7 +22393,7 @@
       </c>
       <c r="F332" t="inlineStr">
         <is>
-          <t>আপুনি আপোনাৰ চোৱা ইণ্ডিয়া &lt;বেজ-ৰং&gt; &lt;span&gt;ভাষা সমাৰ্থক&lt;/span&gt; বেজ অৰ্জন কৰিছে৷</t>
+          <t>আপুনি আপোনাৰ চোৱা ইণ্ডিয়া &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt;ভাষা সমাৰ্থক&lt;/span&gt; বেজ অৰ্জন কৰিছে৷</t>
         </is>
       </c>
       <c r="G332" t="inlineStr">
@@ -22450,58 +22450,58 @@
       </c>
       <c r="C333" t="inlineStr">
         <is>
-          <t>आपने अपना देखो इंडिया &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt;भाषा समर्थक बैज&lt;/span&gt; अर्जित किया है।</t>
+          <t>आपने अपना लिखो इंडिया &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt;भाषा समर्थक&lt;/span&gt; बैज अर्जित किया है।</t>
         </is>
       </c>
       <c r="D333" t="inlineStr"/>
       <c r="E333" t="inlineStr">
         <is>
-          <t>તમે તમારું જુવો ઇન્ડિયા &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt;ભાષા સમર્થક&lt;/span&gt; બેજેસ મેળવીયા છે.</t>
+          <t>તમે તમારું લખો ઇન્ડિયા &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt;ભાષા સમર્થક&lt;/span&gt; બેજ મેળવ્યુ છે .</t>
         </is>
       </c>
       <c r="F333" t="inlineStr">
         <is>
-          <t>আপুনি আপোনাৰ চোৱা ইণ্ডিয়া &lt;বেজ-ৰং&gt; &lt;span&gt;ভাষা সমাৰ্থক&lt;/span&gt; বেজ অৰ্জন কৰিছে৷</t>
+          <t>আপুনি আপোনাৰ লিখা ইণ্ডিয়া &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt;ভাষা সমাৰ্থক&lt;/span&gt; বেজ অৰ্জন কৰিছে৷</t>
         </is>
       </c>
       <c r="G333" t="inlineStr">
         <is>
-          <t>আপনি আপনার দেখো ইন্ডিয়া &lt;span&gt;{{badge}}&lt;/span&gt;  &lt;span&gt;ভাষা সমর্থক&lt;/span&gt; ব্যাজ অর্জন করেছেন।</t>
+          <t>আপনি আপনার লেখো ইন্ডিয়া &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt;ভাষা সমর্থক&lt;/span&gt; ব্যাজ অর্জন করেছেন।</t>
         </is>
       </c>
       <c r="H333" t="inlineStr">
         <is>
-          <t>நீங்கள் உங்கள் பார் இந்தியா &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt;பாஷா சமர்த்தக்&lt;/span&gt; பேட்ஜைப் பெற்றுள்ளீர்கள்.</t>
+          <t>உங்கள் எழுது இந்தியா &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt;பாஷா சமர்த்தக் பேட்ஜை&lt;/span&gt; நீங்கள் பெற்றுள்ளீர்கள்.</t>
         </is>
       </c>
       <c r="I333" t="inlineStr">
         <is>
-          <t>మీరు చూడు ఇండియా &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt;భాషా సమర్థక్&lt;/span&gt; బ్యాడ్జ్ సంపాదించారు.</t>
+          <t>మీరు వ్రాయి ఇండియా &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt;భాషా సమార్థక్&lt;/span&gt; బ్యాడ్జ్ సంపాదించారు.</t>
         </is>
       </c>
       <c r="J333" t="inlineStr">
         <is>
-          <t>तुम्ही तुमचा पहा इंडिया &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt;भाषा समर्थक&lt;/span&gt; बॅज प्राप्त केला आहे.</t>
+          <t>तुम्ही तुमचा लिही इंडिया &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt;भाषा समर्थक&lt;/span&gt; बॅज प्राप्त केला आहे.</t>
         </is>
       </c>
       <c r="K333" t="inlineStr">
         <is>
-          <t>ਤੁਸੀਂ ਆਪਣਾ ਦੇਖੋ ਇੰਡੀਆ &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt; ਭਾਸ਼ਾ ਸਮਰਥਕ ਬੈਜ &lt;/span&gt; ਪ੍ਰਾਪਤ ਕੀਤਾ ਹੈ।</t>
+          <t>ਤੁਸੀਂ ਆਪਣਾ ਲਿਖੋ ਇੰਡੀਆ &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt;ਭਾਸ਼ਾ ਸਮਰਥਕ&lt;/span&gt; ਬੈਜ ਪ੍ਰਾਪਤ ਕੀਤਾ ਹੈ।</t>
         </is>
       </c>
       <c r="L333" t="inlineStr">
         <is>
-          <t>നിങ്ങള്‍ കാണുക ഇന്ത്യ &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt;ഭാഷാ സമര്‍ത്ഥക്&lt;/span&gt; ബാഡ്ജ് നേടിയിരിക്കുന്നു.</t>
+          <t>താങ്കള്‍ എഴുതൂ ഇന്ത്യ &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt;ഭാഷാ സമര്‍ത്ഥക്&lt;/span&gt; ബാഡ്ജ് നേടിയിരിക്കുന്നു.</t>
         </is>
       </c>
       <c r="M333" t="inlineStr">
         <is>
-          <t>ଆପଣ ନିଜର ଦେଖ ଇଣ୍ଡିଆ &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt;ଭାଷା ସମର୍ଥକ&lt;/span&gt; ବ୍ୟାଜ ଅର୍ଜନ କରିଛନ୍ତି।</t>
+          <t>ଆପଣ ନିଜର ଲେଖ ଇଣ୍ଡିଆ &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt;ଭାଷା ସମର୍ଥକ&lt;/span&gt; ବ୍ୟାଜ ଅର୍ଜନ କରିଛନ୍ତି।</t>
         </is>
       </c>
       <c r="N333" t="inlineStr">
         <is>
-          <t>ನೀವು ನಿಮ್ಮ ನೋಡು ಇಂಡಿಯಾ &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt; ಭಾಷಾ ಸಮರ್ಥಕ್  &lt;/span&gt; ಬ್ಯಾಡ್ಜ್ ಅನ್ನು ಗಳಿಸಿದ್ದೀರಿ.</t>
+          <t>ನೀವು ನಿಮ್ಮ ಬರೆ ಇಂಡಿಯಾ &lt;span&gt;{{badge}}&lt;/span&gt; &lt;span&gt; ಭಾಷಾ ಸಮರ್ಥಕ್ &lt;/span&gt; ಬ್ಯಾಡ್ಜ್ ಅನ್ನು ಗಳಿಸಿದ್ದೀರಿ.</t>
         </is>
       </c>
     </row>
@@ -22529,7 +22529,7 @@
       </c>
       <c r="F334" t="inlineStr">
         <is>
-          <t>&lt;ভাষা&gt;ত &lt;অৰিহণা-গণনা&gt; &lt;strong&gt;ৰেকৰ্ডিং(বোৰ)ৰ &lt;/strong&gt; অৰিহণা আগবঢ়োৱা হৈছে৷</t>
+          <t>{{language}}ত &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt;ৰেকৰ্ডিং(বোৰ)ৰ &lt;/strong&gt; অৰিহণা আগবঢ়োৱা হৈছে৷</t>
         </is>
       </c>
       <c r="G334" t="inlineStr">
@@ -22597,7 +22597,7 @@
       </c>
       <c r="F335" t="inlineStr">
         <is>
-          <t>প্ৰতিলিপিকৃত &lt;অৰিহনা-গণনা&gt; &lt;strong&gt;বাক্য&lt;/strong&gt; &lt;ভাষা&gt;ত</t>
+          <t>প্ৰতিলিপিকৃত &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt;বাক্য&lt;/strong&gt; {{language}}ত</t>
         </is>
       </c>
       <c r="G335" t="inlineStr">
@@ -22665,7 +22665,7 @@
       </c>
       <c r="F336" t="inlineStr">
         <is>
-          <t>&lt;ভাষা&gt;ত &lt;অৰিহণা-গণনা&gt; &lt;strong&gt; ছবিৰ লেবেল (সমূহ) &lt;/strong&gt;প্ৰতিলিপিকৃত হৈছে৷</t>
+          <t>{{language}}ত &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt; ছবিৰ লেবেল (সমূহ) &lt;/strong&gt;প্ৰতিলিপিকৃত হৈছে৷</t>
         </is>
       </c>
       <c r="G336" t="inlineStr">
@@ -22733,7 +22733,7 @@
       </c>
       <c r="F337" t="inlineStr">
         <is>
-          <t>অনুবাদকৃত &lt;অৰিহণা-গণনা&gt; &lt;ভাষা&gt; &lt;strong&gt;বাক্য(বোৰ)&lt;/strong&gt;</t>
+          <t>অনুবাদকৃত &lt;strong&gt;{{count}}&lt;/strong&gt; {{language}} &lt;strong&gt;বাক্য(বোৰ)&lt;/strong&gt;</t>
         </is>
       </c>
       <c r="G337" t="inlineStr">
@@ -22801,7 +22801,7 @@
       </c>
       <c r="F338" t="inlineStr">
         <is>
-          <t>&lt;ভাষা&gt;ত বৈধতা প্ৰদান কৰা &lt;অৰিহণাৰ-গণনা&gt; &lt;strong&gt;বাক্য(বোৰ)&lt;/strong&gt;</t>
+          <t>{{language}}ত বৈধতা প্ৰদান কৰা &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt;বাক্য(বোৰ)&lt;/strong&gt;</t>
         </is>
       </c>
       <c r="G338" t="inlineStr">
@@ -22869,7 +22869,7 @@
       </c>
       <c r="F339" t="inlineStr">
         <is>
-          <t>&lt;ভাষা&gt;ত বৈধতা প্ৰদান কৰা &lt;অৰিহণাৰ-গণনা&gt; &lt;strong&gt;বাক্য(বোৰ)&lt;/strong&gt;</t>
+          <t>{{language}}ত বৈধতা প্ৰদান কৰা &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt;বাক্য(বোৰ)&lt;/strong&gt;</t>
         </is>
       </c>
       <c r="G339" t="inlineStr">
@@ -22937,7 +22937,7 @@
       </c>
       <c r="F340" t="inlineStr">
         <is>
-          <t>&lt;ভাষা&gt;ত &lt;অৰিহণা-গণনা&gt; &lt;strong&gt; ছবিৰ লেবেল (বোৰ)ক &lt;/strong&gt; বৈধতা প্ৰদান কৰা হৈছে৷</t>
+          <t>{{language}}ত &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt; ছবিৰ লেবেল (বোৰ)ক &lt;/strong&gt; বৈধতা প্ৰদান কৰা হৈছে৷</t>
         </is>
       </c>
       <c r="G340" t="inlineStr">
@@ -23005,7 +23005,7 @@
       </c>
       <c r="F341" t="inlineStr">
         <is>
-          <t>বৈধতা প্ৰদান কৰা&lt;অৰিহণা-গণনা&gt; &lt;ভাষা&gt; &lt;strong&gt;বাক্য(বোৰ)&lt;/strong&gt;</t>
+          <t>বৈধতা প্ৰদান কৰা &lt;strong&gt;{{count}}&lt;/strong&gt; {{language}} &lt;strong&gt;বাক্য(বোৰ)&lt;/strong&gt;</t>
         </is>
       </c>
       <c r="G341" t="inlineStr">
@@ -23062,7 +23062,7 @@
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>अपना {{nextBadgeType}}  बैज अर्जित करने के लिए &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt;रिकॉर्डिंग्स&lt;s/&gt; का योगदान दें।</t>
+          <t>अपना {{nextBadgeType}}  बैज अर्जित करने के लिए &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt;रिकॉर्डिंग्स&lt;/strong&gt; का योगदान दें।</t>
         </is>
       </c>
       <c r="D342" t="inlineStr"/>
@@ -23073,7 +23073,7 @@
       </c>
       <c r="F342" t="inlineStr">
         <is>
-          <t>আপোনাৰ &lt;বেজ- ৰং&gt; বেজ অৰ্জন কৰিবলৈ &lt;অৰিহণা- গণনা&gt; &lt;strong&gt;ৰেকৰ্ডিংটো(বোৰ)&lt;/strong&gt; অৰিহনা আগবঢ়াওক৷</t>
+          <t>আপোনাৰ {{nextBadgeType}} বেজ অৰ্জন কৰিবলৈ &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt;ৰেকৰ্ডিংটো(বোৰ)&lt;/strong&gt; অৰিহনা আগবঢ়াওক৷</t>
         </is>
       </c>
       <c r="G342" t="inlineStr">
@@ -23141,7 +23141,7 @@
       </c>
       <c r="F343" t="inlineStr">
         <is>
-          <t>আপোনাৰ &lt;বেজ- ৰং&gt; বেজ অৰ্জন কৰিবলৈ &lt;অৰিহণা- গণনা&gt; &lt;strong&gt;বাক্যটো(বোৰ)&lt;/strong&gt; অৰিহনা আগবঢ়াওক৷</t>
+          <t>আপোনাৰ {{nextBadgeType}} বেজ অৰ্জন কৰিবলৈ &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt;বাক্যটো(বোৰ)&lt;/strong&gt; অৰিহনা আগবঢ়াওক৷</t>
         </is>
       </c>
       <c r="G343" t="inlineStr">
@@ -23209,7 +23209,7 @@
       </c>
       <c r="F344" t="inlineStr">
         <is>
-          <t>আপোনাৰ &lt;বেজ- ৰং&gt; বেজ অৰ্জন কৰিবলৈ &lt;অৰিহণা- গণনা&gt; &lt;strong&gt;ছবিৰ লেবেল (সমূহ)&lt;/strong&gt; অৰিহনা আগবঢ়াওক৷</t>
+          <t>আপোনাৰ {{nextBadgeType}} বেজ অৰ্জন কৰিবলৈ &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt;ছবিৰ লেবেল (সমূহ)&lt;/strong&gt; অৰিহনা আগবঢ়াওক৷</t>
         </is>
       </c>
       <c r="G344" t="inlineStr">
@@ -23277,7 +23277,7 @@
       </c>
       <c r="F345" t="inlineStr">
         <is>
-          <t>আপোনাৰ &lt;বেজ- ৰং&gt; বেজ অৰ্জন কৰিবলৈ &lt;অৰিহণা- গণনা&gt; &lt;strong&gt;বাক্যটো(বোৰ)&lt;/strong&gt; অৰিহনা আগবঢ়াওক৷</t>
+          <t>আপোনাৰ {{nextBadgeType}} বেজ অৰ্জন কৰিবলৈ &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt;বাক্যটো(বোৰ)&lt;/strong&gt; অৰিহনা আগবঢ়াওক৷</t>
         </is>
       </c>
       <c r="G345" t="inlineStr">
@@ -23332,18 +23332,62 @@
           <t>Validate &lt;contribution-count&gt; &lt;s&gt;sentence(s)&lt;/s&gt; to earn your &lt;badge-color&gt; Badge.</t>
         </is>
       </c>
-      <c r="C346" t="inlineStr"/>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>अपना {{nextBadgeType}} बैज जीतने के लिए &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt;वाक्यों&lt;/strong&gt; को सत्यापित करें।</t>
+        </is>
+      </c>
       <c r="D346" t="inlineStr"/>
-      <c r="E346" t="inlineStr"/>
-      <c r="F346" t="inlineStr"/>
-      <c r="G346" t="inlineStr"/>
-      <c r="H346" t="inlineStr"/>
-      <c r="I346" t="inlineStr"/>
-      <c r="J346" t="inlineStr"/>
-      <c r="K346" t="inlineStr"/>
-      <c r="L346" t="inlineStr"/>
-      <c r="M346" t="inlineStr"/>
-      <c r="N346" t="inlineStr"/>
+      <c r="E346" t="inlineStr">
+        <is>
+          <t>{{nextBadgeType}} બેજ મેળવવા માટે &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt;વાક્યોને&lt;/strong&gt; વેલિડેટ કરો ।</t>
+        </is>
+      </c>
+      <c r="F346" t="inlineStr">
+        <is>
+          <t>আপোনাৰ {{nextBadgeType}} বেজ অৰ্জন কৰিবলৈ &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt;বাক্যটো (সমূহ)&lt;/strong&gt; বৈধতা প্ৰদান কৰক৷</t>
+        </is>
+      </c>
+      <c r="G346" t="inlineStr">
+        <is>
+          <t>{{nextBadgeType}} ব্যাজ অর্জন করার জন্য &lt;strong&gt;{{count}}&lt;/strong&gt; টি &lt;strong&gt;বাক্য&lt;/strong&gt; যাচাই করুন।</t>
+        </is>
+      </c>
+      <c r="H346" t="inlineStr">
+        <is>
+          <t>உங்கள் {{nextBadgeType}} பேட்ஜைப் பெற &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt;வாக்கியங்களை&lt;/strong&gt; சரிபார்க்கவும்.</t>
+        </is>
+      </c>
+      <c r="I346" t="inlineStr">
+        <is>
+          <t>మీ {{nextBadgeType}} బ్యాడ్జ్ సంపాదించడానికి &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt;వాక్యాలను&lt;/strong&gt; ధృవీకరించండి.</t>
+        </is>
+      </c>
+      <c r="J346" t="inlineStr">
+        <is>
+          <t>तुमचा  {{nextBadgeType}} बॅज प्राप्त करण्यासाठी  &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt;वाक्यांना&lt;/strong&gt; प्रमाणित करा.</t>
+        </is>
+      </c>
+      <c r="K346" t="inlineStr">
+        <is>
+          <t>ਆਪਣਾ {{nextBadgeType}}ਬੈਜ ਪ੍ਰਾਪਤ ਕਰਨ ਲਈ &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt;ਵਾਕਾਂ&lt;/strong&gt; ਨੂੰ ਪ੍ਰਮਾਣਿਤ ਕਰੋ।</t>
+        </is>
+      </c>
+      <c r="L346" t="inlineStr">
+        <is>
+          <t>{{nextBadgeType}} ബാഡ്ജ് നേടുന്നതിനായി &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt;വാക്യങ്ങള്‍&lt;/strong&gt; സാധൂകരിക്കുക.</t>
+        </is>
+      </c>
+      <c r="M346" t="inlineStr">
+        <is>
+          <t>{{nextBadgeType}} ବ୍ୟାଜ ଅର୍ଜନ କରିବା ପାଇଁ &lt;strong&gt;{{count}}&lt;/strong&gt;ଟି &lt;strong&gt;ବାକ୍ୟର&lt;/strong&gt; ପ୍ରାମାଣିକତା ସାବ୍ୟସ୍ତ କରନ୍ତୁ।</t>
+        </is>
+      </c>
+      <c r="N346" t="inlineStr">
+        <is>
+          <t>ನಿಮ್ಮ {{nextBadgeType}} ಬ್ಯಾಡ್ಜ್ ಅನ್ನು ಗಳಿಸಲು &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt; ವಾಕ್ಯಗಳನ್ನು &lt;/strong&gt;  ಮೌಲ್ಯೀಕರಿಸಿ.</t>
+        </is>
+      </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
@@ -23369,7 +23413,7 @@
       </c>
       <c r="F347" t="inlineStr">
         <is>
-          <t>আপোনাৰ &lt;বেজ- ৰং&gt; বেজ অৰ্জন কৰিবলৈ &lt;অৰিহণা- গণনা&gt; &lt;strong&gt;বাক্যটো (সমূহ)&lt;/strong&gt; বৈধতা প্ৰদান কৰক৷</t>
+          <t>আপোনাৰ {{nextBadgeType}} বেজ অৰ্জন কৰিবলৈ &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt;বাক্যটো (সমূহ)&lt;/strong&gt; বৈধতা প্ৰদান কৰক৷</t>
         </is>
       </c>
       <c r="G347" t="inlineStr">
@@ -23437,7 +23481,7 @@
       </c>
       <c r="F348" t="inlineStr">
         <is>
-          <t>আপোনাৰ &lt;বেজ- ৰং&gt; বেজ অৰ্জন কৰিবলৈ &lt;অৰিহণা- গণনা&gt; &lt;strong&gt;ছবিৰ লেবেল (সমূহ)ক &lt;/strong&gt; বৈধতা প্ৰদান কৰক৷</t>
+          <t>আপোনাৰ {{nextBadgeType}} বেজ অৰ্জন কৰিবলৈ &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt;ছবিৰ লেবেল (সমূহ)ক &lt;/strong&gt; বৈধতা প্ৰদান কৰক৷</t>
         </is>
       </c>
       <c r="G348" t="inlineStr">
@@ -23505,7 +23549,7 @@
       </c>
       <c r="F349" t="inlineStr">
         <is>
-          <t>আপোনাৰ &lt;বেজ- ৰং&gt; বেজ অৰ্জন কৰিবলৈ &lt;অৰিহণা- গণনা&gt; &lt;strong&gt;বাক্যটো (সমূহ)&lt;/strong&gt; বৈধতা প্ৰদান কৰক৷</t>
+          <t>আপোনাৰ {{nextBadgeType}} বেজ অৰ্জন কৰিবলৈ &lt;strong&gt;{{count}}&lt;/strong&gt; &lt;strong&gt;বাক্যটো (সমূহ)&lt;/strong&gt; বৈধতা প্ৰদান কৰক৷</t>
         </is>
       </c>
       <c r="G349" t="inlineStr">
@@ -23573,7 +23617,7 @@
       </c>
       <c r="F350" t="inlineStr">
         <is>
-          <t>&lt;ভাষা&gt; বনাম শীৰ্ষ অৰিহণা আগবঢ়োৱা ভাষা</t>
+          <t>{{language}} বনাম শীৰ্ষ অৰিহণা আগবঢ়োৱা ভাষা</t>
         </is>
       </c>
       <c r="G350" t="inlineStr">
@@ -23641,7 +23685,7 @@
       </c>
       <c r="F351" t="inlineStr">
         <is>
-          <t>&lt;ভাষা&gt; বনাম শীৰ্ষ অৰিহণা আগবঢ়োৱা ভাষা</t>
+          <t>{{language}} বনাম শীৰ্ষ অৰিহণা আগবঢ়োৱা ভাষা</t>
         </is>
       </c>
       <c r="G351" t="inlineStr">
@@ -23709,7 +23753,7 @@
       </c>
       <c r="F352" t="inlineStr">
         <is>
-          <t>&lt;ভাষা&gt; বনাম শীৰ্ষ অৰিহণা আগবঢ়োৱা ভাষা</t>
+          <t>{{language}} বনাম শীৰ্ষ অৰিহণা আগবঢ়োৱা ভাষা</t>
         </is>
       </c>
       <c r="G352" t="inlineStr">
@@ -23772,12 +23816,12 @@
       <c r="D353" t="inlineStr"/>
       <c r="E353" t="inlineStr">
         <is>
-          <t>&lt;from-language&gt; -  &lt;to-language&gt; વિરૃદ્ધ સૌથી વધુ યોગદાન વાળી ભાષા જોડી</t>
+          <t>{{language}} વિરૃદ્ધ સૌથી વધુ યોગદાન વાળી ભાષા જોડી</t>
         </is>
       </c>
       <c r="F353" t="inlineStr">
         <is>
-          <t>&lt;ভাষাৰ-পৰা&gt;-&lt;ভাষা-লৈ&gt; বনাম শীৰ্ষ অৱদানকাৰী ভাষা যোৰ</t>
+          <t>{{language}} বনাম শীৰ্ষ অৱদানকাৰী ভাষা যোৰ</t>
         </is>
       </c>
       <c r="G353" t="inlineStr">
@@ -23802,7 +23846,7 @@
       </c>
       <c r="K353" t="inlineStr">
         <is>
-          <t>&lt;from-language&gt; -  &lt;to-language&gt; ਬਨਾਮ ਚੋਟੀ ਦੀਆਂ ਯੋਗਦਾਨ ਪਾਉਣ ਵਾਲੀਆਂ ਭਾਸ਼ਾ ਜੋੜੀਆਂ</t>
+          <t>{{language}} ਬਨਾਮ ਚੋਟੀ ਦੀਆਂ ਯੋਗਦਾਨ ਪਾਉਣ ਵਾਲੀਆਂ ਭਾਸ਼ਾ ਜੋੜੀਆਂ</t>
         </is>
       </c>
       <c r="L353" t="inlineStr">
@@ -23913,7 +23957,7 @@
       </c>
       <c r="F355" t="inlineStr">
         <is>
-          <t>&lt;উদ্যোগ&gt;ৰ বাবে কোনো বেজ অৰ্জন কৰা নাই</t>
+          <t>{{initiativeName}} ৰ বাবে কোনো বেজ অৰ্জন কৰা নাই</t>
         </is>
       </c>
       <c r="G355" t="inlineStr">
@@ -23986,7 +24030,7 @@
       </c>
       <c r="G356" t="inlineStr">
         <is>
-          <t>স্বীকৃতি পেতে হলে অনুগ্রহ করে সক্রিয়ভাবে যোগদান দিতে থাকুন ।</t>
+          <t>স্বীকৃতি পেতে হলে অনুগ্রহ করে সক্রিয়ভাবে যোগদান দিতে থাকুন।</t>
         </is>
       </c>
       <c r="H356" t="inlineStr">
@@ -24321,7 +24365,7 @@
       </c>
       <c r="F361" t="inlineStr">
         <is>
-          <t>আপুনি এগৰাকী &lt;বেজ-ৰং&gt; অৱদানকাৰী</t>
+          <t>আপুনি এগৰাকী &lt;span&gt;{{badgeType}}&lt;/span&gt; অৱদানকাৰী</t>
         </is>
       </c>
       <c r="G361" t="inlineStr">
@@ -24389,7 +24433,7 @@
       </c>
       <c r="F362" t="inlineStr">
         <is>
-          <t>আপুনি এগৰাকী &lt;বেজ-ৰং&gt; বৈধতা প্ৰদানকাৰী</t>
+          <t>আপুনি এগৰাকী &lt;span&gt;{{badgeType}}&lt;/span&gt; বৈধতা প্ৰদানকাৰী</t>
         </is>
       </c>
       <c r="G362" t="inlineStr">
@@ -24446,7 +24490,7 @@
       </c>
       <c r="C363" t="inlineStr">
         <is>
-          <t>ऑडियो सुनते हुए टेक्स्ट  टाइप करें</t>
+          <t>ऑडियो सुनते हुए टेक्स्ट टाइप करें</t>
         </is>
       </c>
       <c r="D363" t="inlineStr"/>
@@ -24686,7 +24730,7 @@
       </c>
       <c r="K366" t="inlineStr">
         <is>
-          <t>ਕੀ ਆਡੀਓ ਟੈਕਸਟ ਨਾਲ ਮੇਲ ਖਾਂਦਾ ਹੈ?</t>
+          <t>ਕੀ ਆਡੀਓ ਟੈਕਸਟ ਨਾਲ ਮੇਲ ਖਾ ਰਿਹਾ ਹੈ?</t>
         </is>
       </c>
       <c r="L366" t="inlineStr">
@@ -24786,7 +24830,7 @@
       </c>
       <c r="C368" t="inlineStr">
         <is>
-          <t>क्या इमेज से टेक्स्ट को सही सही लिया  गया है?</t>
+          <t>क्या इमेज से टेक्स्ट को सही सही लिया गया है?</t>
         </is>
       </c>
       <c r="D368" t="inlineStr"/>
@@ -24865,7 +24909,7 @@
       </c>
       <c r="F369" t="inlineStr">
         <is>
-          <t>How can you win Bhasha Samarthak Badges</t>
+          <t>আপুনি কেনেদৰে ভাষা সমৰ্থক বেজ সমূহ জিকিব পাৰিব</t>
         </is>
       </c>
       <c r="G369" t="inlineStr">
@@ -24933,7 +24977,7 @@
       </c>
       <c r="F370" t="inlineStr">
         <is>
-          <t>Your Language</t>
+          <t>আপোনাৰ ভাষা</t>
         </is>
       </c>
       <c r="G370" t="inlineStr">
@@ -25001,7 +25045,7 @@
       </c>
       <c r="F371" t="inlineStr">
         <is>
-          <t>Select Badge level</t>
+          <t>বেজৰ স্তৰ বাচি লওক</t>
         </is>
       </c>
       <c r="G371" t="inlineStr">
@@ -25069,7 +25113,7 @@
       </c>
       <c r="F372" t="inlineStr">
         <is>
-          <t>Participation</t>
+          <t>অংশগ্ৰহণ</t>
         </is>
       </c>
       <c r="G372" t="inlineStr">
@@ -25094,7 +25138,7 @@
       </c>
       <c r="K372" t="inlineStr">
         <is>
-          <t>ਹਿੱਸਾ ਲੈਣਾ</t>
+          <t>ਭਾਗੀਦਾਰੀ</t>
         </is>
       </c>
       <c r="L372" t="inlineStr">
@@ -25126,58 +25170,58 @@
       </c>
       <c r="C373" t="inlineStr">
         <is>
-          <t>{{language}} में &lt;span&gt;{{count}} {{sourceType}}&lt;/span&gt; {{action}} और {{initiativeName}} {{badge}} भाषा समर्थक बैज अर्जित करें</t>
+          <t>{{language}} में &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt;{{sourceType}}&lt;/span&gt; {{action}} और {{initiativeName}} {{badge}} भाषा समर्थक बैज अर्जित करें</t>
         </is>
       </c>
       <c r="D373" t="inlineStr"/>
       <c r="E373" t="inlineStr">
         <is>
-          <t>{{language}} માં   &lt;span&gt;{{count}} {{sourceType}}&lt;/span&gt; {{action}} અને  {{initiativeName}} {{badge}} ભાષા સમર્થક બેજ મેળવો .</t>
+          <t>{{language}} માં   &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt;{{sourceType}}&lt;/span&gt; {{action}} અને  {{initiativeName}} {{badge}} ભાષા સમર્થક બેજ મેળવો .</t>
         </is>
       </c>
       <c r="F373" t="inlineStr">
         <is>
-          <t>&lt;ভাষা&gt;ত &lt;অংশগ্ৰহণৰ-প্ৰকাৰ&gt; &lt;মাইলষ্টোন&gt; &lt;পাঠৰ-প্ৰকাৰ&gt;  আৰু  &lt;উদ্যোগ&gt; &lt;বেজৰ-ৰং&gt; ভাষা সমাৰ্থক বেজ অৰ্জন কৰক৷</t>
+          <t>{{language}}ত {{action}} &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt;{{sourceType}}&lt;/span&gt;  আৰু  {{initiativeName}} {{badge}} ভাষা সমাৰ্থক বেজ অৰ্জন কৰক৷</t>
         </is>
       </c>
       <c r="G373" t="inlineStr">
         <is>
-          <t>{{language}} তে  &lt;span&gt;{{count}} {{sourceType}}&lt;/span&gt; {{action}}  করুন এবং {{initiativeName}} {{badge}} ভাষা সমর্থক ব্যাজ অর্জন করুন</t>
+          <t>{{language}} তে  &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt;{{sourceType}}&lt;/span&gt; {{action}}  করুন এবং {{initiativeName}} {{badge}} ভাষা সমর্থক ব্যাজ অর্জন করুন</t>
         </is>
       </c>
       <c r="H373" t="inlineStr">
         <is>
-          <t>{{language}} இல் {{action}} &lt;span&gt;{{count}} {{sourceType}}&lt;/span&gt; மற்றும் {{initiativeName}} {{badge}} பாஷா சமர்த்தக் பேட்ஜைப் பெறுங்கள்</t>
+          <t>{{language}} இல் {{action}} &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt;{{sourceType}}&lt;/span&gt; மற்றும் {{initiativeName}} {{badge}} பாஷா சமர்த்தக் பேட்ஜைப் பெறுங்கள்</t>
         </is>
       </c>
       <c r="I373" t="inlineStr">
         <is>
-          <t>{{language}} లో  &lt;span&gt;{{count}} {{sourceType}}&lt;/span&gt; {{action}} చేయండి మరియు {{initiativeName}} {{badge}} భాషా సమార్థక్ బ్యాడ్జ్ సంపాదించండి</t>
+          <t>{{language}} లో  &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt;{{sourceType}}&lt;/span&gt; {{action}} చేయండి మరియు {{initiativeName}} {{badge}} భాషా సమార్థక్ బ్యాడ్జ్ సంపాదించండి</t>
         </is>
       </c>
       <c r="J373" t="inlineStr">
         <is>
-          <t>{{language}} मध्ये  &lt;span&gt;{{count}} {{sourceType}}&lt;/span&gt; {{action}} आणि {{initiativeName}} {{badge}}  भाषा समर्थक बॅज मिळवा</t>
+          <t>{{language}} मध्ये  &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt;{{sourceType}}&lt;/span&gt; {{action}} आणि {{initiativeName}} {{badge}}  भाषा समर्थक बॅज मिळवा</t>
         </is>
       </c>
       <c r="K373" t="inlineStr">
         <is>
-          <t>{{language}} ਵਿੱਚ &lt;span&gt;{{count}} {{sourceType}}&lt;/span&gt; {{action}} ਅਤੇ {{initiativeName}} {{badge}} ਭਾਸ਼ਾ ਸਮਰਥਕ ਬੈਜ ਪ੍ਰਾਪਤ ਕਰੋ</t>
+          <t>{{language}} ਵਿੱਚ &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt;{{sourceType}}&lt;/span&gt; {{action}} ਅਤੇ {{initiativeName}} {{badge}} ਭਾਸ਼ਾ ਸਮਰਥਕ ਬੈਜ ਪ੍ਰਾਪਤ ਕਰੋ</t>
         </is>
       </c>
       <c r="L373" t="inlineStr">
         <is>
-          <t>{{language}}-ല്‍ {{action}} &lt;span&gt;{{count}} {{sourceType}}&lt;/span&gt; ചെയ്യൂ {{initiativeName}} {{badge}} ഭാഷാ സമര്‍ത്ഥക് ബാഡ്ജ് നേടൂ</t>
+          <t>{{language}}-ല്‍ {{action}} &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt;{{sourceType}}&lt;/span&gt; ചെയ്യൂ {{initiativeName}} {{badge}} ഭാഷാ സമര്‍ത്ഥക് ബാഡ്ജ് നേടൂ</t>
         </is>
       </c>
       <c r="M373" t="inlineStr">
         <is>
-          <t>{{language}}ରେ {{action}} &lt;span&gt;{{count}} {{sourceType}}&lt;/span&gt; ଏବଂ {{initiativeName}} {{badge}} ଭାଷା ସମର୍ଥକ ବ୍ୟାଜ ଅର୍ଜନ କରନ୍ତୁ</t>
+          <t>{{language}}ରେ {{action}} &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt;{{sourceType}}&lt;/span&gt; ଏବଂ {{initiativeName}} {{badge}} ଭାଷା ସମର୍ଥକ ବ୍ୟାଜ ଅର୍ଜନ କରନ୍ତୁ</t>
         </is>
       </c>
       <c r="N373" t="inlineStr">
         <is>
-          <t>{{language}} ಭಾಷೆಯಲ್ಲಿ  &lt;span&gt;{{count}} {{sourceType}}&lt;/span&gt; {{action}}  ಮಾಡಿ ಮತ್ತು  {{initiativeName}} {{badge}} ಭಾಷಾ ಸಮರ್ಥಕ್ ಬ್ಯಾಡ್ಜ್ ಅನ್ನು ಗಳಿಸಿ.</t>
+          <t>{{language}} ಭಾಷೆಯಲ್ಲಿ  &lt;span&gt;{{count}}&lt;/span&gt; &lt;span&gt;{{sourceType}}&lt;/span&gt; {{action}}  ಮಾಡಿ ಮತ್ತು  {{initiativeName}} {{badge}} ಭಾಷಾ ಸಮರ್ಥಕ್ ಬ್ಯಾಡ್ಜ್ ಅನ್ನು ಗಳಿಸಿ.</t>
         </is>
       </c>
     </row>
@@ -25210,7 +25254,7 @@
       </c>
       <c r="G374" t="inlineStr">
         <is>
-          <t>শুধুমাত্র ১০০০টি অক্ষর অনুমোদিত</t>
+          <t>কেবল ১০০০ টি অক্ষর অনুমোদিত</t>
         </is>
       </c>
       <c r="H374" t="inlineStr">
@@ -25225,12 +25269,12 @@
       </c>
       <c r="J374" t="inlineStr">
         <is>
-          <t>फक्त १२ वर्णांची संभावना</t>
+          <t>फक्त 1000 वर्णांची अनुमती</t>
         </is>
       </c>
       <c r="K374" t="inlineStr">
         <is>
-          <t>ਸਿਰਫ 1000 ਅੱਖਰਾਂ ਦੀ ਇਜਾਜ਼ਤ ਹੈ</t>
+          <t>ਸਿਰਫ 1000 ਅੱਖਰਾਂ ਦੀ ਇਜਾਜ਼ਤ</t>
         </is>
       </c>
       <c r="L374" t="inlineStr">
@@ -25240,7 +25284,7 @@
       </c>
       <c r="M374" t="inlineStr">
         <is>
-          <t xml:space="preserve">କେବଳ 1000 ଅକ୍ଷର ହିଁ ସମ୍ଭବ </t>
+          <t>କେବଳ 1000 ଅକ୍ଷର ହିଁ ସମ୍ଭବ</t>
         </is>
       </c>
       <c r="N374" t="inlineStr">
@@ -25376,18 +25420,62 @@
           <t>Test your Microphone and Speakers</t>
         </is>
       </c>
-      <c r="C378" t="inlineStr"/>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>अपने माइक्रोफ़ोन और स्पीकर की जांच कर लें</t>
+        </is>
+      </c>
       <c r="D378" t="inlineStr"/>
-      <c r="E378" t="inlineStr"/>
-      <c r="F378" t="inlineStr"/>
-      <c r="G378" t="inlineStr"/>
-      <c r="H378" t="inlineStr"/>
-      <c r="I378" t="inlineStr"/>
-      <c r="J378" t="inlineStr"/>
-      <c r="K378" t="inlineStr"/>
-      <c r="L378" t="inlineStr"/>
-      <c r="M378" t="inlineStr"/>
-      <c r="N378" t="inlineStr"/>
+      <c r="E378" t="inlineStr">
+        <is>
+          <t>તમારું માઇક્રોફોન અને સ્પીકર્સ તપાસો</t>
+        </is>
+      </c>
+      <c r="F378" t="inlineStr">
+        <is>
+          <t>আপোনাৰ মাইক্ৰ'ফোন আৰু স্পীকাৰ পৰীক্ষা কৰক</t>
+        </is>
+      </c>
+      <c r="G378" t="inlineStr">
+        <is>
+          <t>আপনার মাইক্রোফোন ও স্পিকার পরীক্ষা করুন</t>
+        </is>
+      </c>
+      <c r="H378" t="inlineStr">
+        <is>
+          <t>உங்கள் ஒலிவாங்கி மற்றும் ஒலிபெருக்கிகளை சோதிக்கவும்</t>
+        </is>
+      </c>
+      <c r="I378" t="inlineStr">
+        <is>
+          <t>మీ మైక్రోఫోన్ మరియు స్పీకర్లను పరీక్షించండి</t>
+        </is>
+      </c>
+      <c r="J378" t="inlineStr">
+        <is>
+          <t>तुमच्या मायक्रोफोन आणि स्पीकर्सची तपासणी करा</t>
+        </is>
+      </c>
+      <c r="K378" t="inlineStr">
+        <is>
+          <t>ਆਪਣੇ ਮਾਈਕ੍ਰੋਫੋਨ ਅਤੇ ਸਪੀਕਰ ਦੀ ਜਾਂਚ ਕਰੋ</t>
+        </is>
+      </c>
+      <c r="L378" t="inlineStr">
+        <is>
+          <t>നിങ്ങളുടെ മൈക്രോഫോണും സ്പീക്കറുകളും പരിശോധിക്കുക</t>
+        </is>
+      </c>
+      <c r="M378" t="inlineStr">
+        <is>
+          <t>ନିଜର ମାଇକ୍ରୋଫୋନ୍ ଏବଂ ସ୍ପିକର୍ କୁ ଯାଞ୍ଚ କରିନିଅନ୍ତୁ</t>
+        </is>
+      </c>
+      <c r="N378" t="inlineStr">
+        <is>
+          <t>ನಿಮ್ಮ ಮೈಕ್ರೋಫೋನ್ ಮತ್ತು ಸ್ಪೀಕರ್‌ಗಳನ್ನು ಪರೀಕ್ಷಿಸಿಕೊಳ್ಳಿ</t>
+        </is>
+      </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
@@ -25796,6 +25884,530 @@
           <t>ತಪ್ಪು</t>
         </is>
       </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>hurtingStatement</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>Hurting sentiments of religion, community or abusive content etc.</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>धर्म, समुदाय की भावनाओं को ठेस पहुँचाने वाला या अपमानजनक कॉन्टेंट</t>
+        </is>
+      </c>
+      <c r="D385" t="inlineStr"/>
+      <c r="E385" t="inlineStr">
+        <is>
+          <t>ધર્મ, સમુદાયની લાગણી દુભાવવી અથવા અપમાનજનક કન્ટેન્ટ વગેરે.</t>
+        </is>
+      </c>
+      <c r="F385" t="inlineStr">
+        <is>
+          <t>ধৰ্ম, সম্প্ৰদায় বা অপমানজনক সমল আদিৰ অনুভুতিত আঘাত কৰা</t>
+        </is>
+      </c>
+      <c r="G385" t="inlineStr">
+        <is>
+          <t>ধর্ম, সম্প্রদায়ের ভাবাদর্শকে আঘাতকারী বা অবমাননাকর বিষয়বস্তু ইত্যাদি</t>
+        </is>
+      </c>
+      <c r="H385" t="inlineStr">
+        <is>
+          <t>மதம், சமூக உணர்வுகளை புண்படுத்துகிற அல்லது திட்டுகிற மாதிரி உள்ளடக்கம் ஆகியவை</t>
+        </is>
+      </c>
+      <c r="I385" t="inlineStr">
+        <is>
+          <t>మతం, సంఘం మనోభావాలను దెబ్బతీయడం లేదా అసభ్యకర విషయాలు మెదలైనవి</t>
+        </is>
+      </c>
+      <c r="J385" t="inlineStr">
+        <is>
+          <t>धर्म, समुदायाच्या भावनांना दुखवणारा किंवा अपमानास्पद मजकूर इ.</t>
+        </is>
+      </c>
+      <c r="K385" t="inlineStr">
+        <is>
+          <t>ਧਰਮ, ਸਮੁਦਾਇ ਦੀਆਂ ਭਾਵਨਾਵਾਂ ਨੂੰ ਠੇਸ ਪਹੁੰਚਾਉਣ ਵਾਲਾ ਜਾਂ ਅਪਮਾਨਜਨਕ ਕੰਟੈਂਟ</t>
+        </is>
+      </c>
+      <c r="L385" t="inlineStr">
+        <is>
+          <t>മതത്തിന്റെയും, സമൂഹത്തിന്റേയും വികാരം വ്രണ പ്പെടുത്തുന്നതോ  അസഭ്യമായ ഉള്ളടക്കമോ മുതലായവ</t>
+        </is>
+      </c>
+      <c r="M385" t="inlineStr">
+        <is>
+          <t>ଧାର୍ମିକ, ସାମ୍ପ୍ରଦାୟିକ ଭାବନାକୁ ଆଘାତ ଦେବା କିମ୍ବା ଅପମାନଜନକ ବିଷୟବସ୍ତୁ ଇତ୍ୟାଦି</t>
+        </is>
+      </c>
+      <c r="N385" t="inlineStr">
+        <is>
+          <t>ಧರ್ಮ, ಸಮುದಾಯಗಳ ಭಾವನೆಗಳನ್ನು ನೋಯಿಸುವ ಅಥವಾ ನಿಂದನೀಯ ಅಂಶಗಳು ಇತ್ಯಾದಿ.</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>hatefulPolitical</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t>Hateful Political views, amplifying hate-speech etc.</t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>नफ़रत फ़ैलाने वाली राजनीतिक सोच, नफ़रत बढ़ाने वाले बयान आदि</t>
+        </is>
+      </c>
+      <c r="D386" t="inlineStr"/>
+      <c r="E386" t="inlineStr">
+        <is>
+          <t>દ્વેષપૂર્ણ રાજકીય મંતવ્યો, ઉશ્કેરણીજનક નિવેદનો વગેરે.</t>
+        </is>
+      </c>
+      <c r="F386" t="inlineStr">
+        <is>
+          <t>ঘৃণনীয় ৰাজনৈতিক মতামত, ঘৃণাৰ-ভাষণ প্ৰচাৰ ইত্যাদি।</t>
+        </is>
+      </c>
+      <c r="G386" t="inlineStr">
+        <is>
+          <t>ঘৃণা উদ্রেককারী রাজনৈতিক মতামত, ঘৃণাবাচক বক্তৃতা ইত্যাদি</t>
+        </is>
+      </c>
+      <c r="H386" t="inlineStr">
+        <is>
+          <t>வெறுக்கத்தக்க அரசியல் கருத்துக்கள், வெறுப்புணர்வை அதிகரிக்கும் பேச்சுரை போன்றவை.</t>
+        </is>
+      </c>
+      <c r="I386" t="inlineStr">
+        <is>
+          <t>ద్వేషపూరిత రాజకీయ అభిప్రాయాలు, ద్వేషపూరిత సంభాషణను ప్రేరేపించడం మొదలైనవి.</t>
+        </is>
+      </c>
+      <c r="J386" t="inlineStr">
+        <is>
+          <t>द्वेषपूर्ण राजकीय मते, भडकावू वक्तव्य इ.</t>
+        </is>
+      </c>
+      <c r="K386" t="inlineStr">
+        <is>
+          <t>ਨਫ਼ਰਤ ਫੈਲਾਉਣ ਵਾਲੀ ਸਿਆਸੀ ਸੋਚ, ਨਫ਼ਰਤ ਵਧਾਉਣ ਵਾਲਾ ਬਿਆਨ ਆਦਿ</t>
+        </is>
+      </c>
+      <c r="L386" t="inlineStr">
+        <is>
+          <t>വെറുപ്പ് നിറഞ്ഞ രാഷ്ട്രീയ കാഴ്ചപ്പാടുകൾ,വിദ്വേഷപ്രചാരണം മുതലായവ</t>
+        </is>
+      </c>
+      <c r="M386" t="inlineStr">
+        <is>
+          <t>ଘୃଣ୍ୟ ରାଜନୈତିକ ଦୃଷ୍ଟିକୋଣ, ଘୃଣା ମନୋଭାବ ବଢ଼େଇଲା ଭଳି ବକ୍ତବ୍ୟ</t>
+        </is>
+      </c>
+      <c r="N386" t="inlineStr">
+        <is>
+          <t>ದ್ವೇಷಪೂರಿತ ರಾಜಕೀಯ ಅಭಿಪ್ರಾಯಗಳು, ದ್ವೇಷವನ್ನು ಉಲ್ಬಣಗೊಳಿಸುವಂತಹ ಹೇಳಿಕೆಗಳು ಇತ್ಯಾದಿ.</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>herseyRumors</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t>Hearsay / Rumors, deliberate falsified facts etc.</t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>सुना सुनाया / अफवाहें, जानबूझकर बताए गए झूठे तथ्य आदि</t>
+        </is>
+      </c>
+      <c r="D387" t="inlineStr"/>
+      <c r="E387" t="inlineStr">
+        <is>
+          <t>ઉડતી વાતો/ અફવાઓ, ઇરાદાપૂર્વક ખોટા ઉભા કરેલા તથ્યો વગેરે</t>
+        </is>
+      </c>
+      <c r="F387" t="inlineStr">
+        <is>
+          <t>শুনা কথা / উৰা-বাতৰি, ইচ্ছাকৃত ভাৱে ভুৱা তথ্য ইত্যাদি।</t>
+        </is>
+      </c>
+      <c r="G387" t="inlineStr">
+        <is>
+          <t>উড়োখবর/গুজব, ইচ্ছাকৃত মিথ্যা তথ্যাদি ইত্যাদি</t>
+        </is>
+      </c>
+      <c r="H387" t="inlineStr">
+        <is>
+          <t>பாசாங்குத்தனம்/வதந்திகள், வேண்டுமென்றே பொய்யான உண்மைகள் போன்றவை.</t>
+        </is>
+      </c>
+      <c r="I387" t="inlineStr">
+        <is>
+          <t>గాలి మాటలు/పుకార్లు, ఉద్దేశపూర్వక తప్పుడు ప్రచారాలు మొదలైనవి.</t>
+        </is>
+      </c>
+      <c r="J387" t="inlineStr">
+        <is>
+          <t>ऐकीव गोष्टी / अफवा, जाणूनबूजून दिलेली खोटी माहिती इ.</t>
+        </is>
+      </c>
+      <c r="K387" t="inlineStr">
+        <is>
+          <t>ਸੁਣੀ-ਸੁਣਾਈ/ਅਫਵਾਹਾਂ, ਜਾਣ-ਬੁੱਝ ਕੇ ਦੱਸੇ ਗਏ ਝੂਠੇ ਤੱਥ ਆਦਿ</t>
+        </is>
+      </c>
+      <c r="L387" t="inlineStr">
+        <is>
+          <t>കേട്ടുകേൾവി/ കിംവദന്തികള്‍, മന:പൂര്‍വ്വം  വളച്ചൊടിച്ച കാര്യങ്ങള്‍</t>
+        </is>
+      </c>
+      <c r="M387" t="inlineStr">
+        <is>
+          <t>ଉଡ଼ନ୍ତା ଖବର / ଗୁଜବ, ସୁଚିନ୍ତିତ ମିଥ୍ୟା ତଥ୍ୟ ଇତ୍ୟାଦି</t>
+        </is>
+      </c>
+      <c r="N387" t="inlineStr">
+        <is>
+          <t>ಗಾಳಿಮಾತುಗಳು / ವದಂತಿಗಳು, ಉದ್ದೇಶಪೂರ್ವಕ ಸುಳ್ಳು ಸಂಗತಿಗಳು ಇತ್ಯಾದಿ.</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>languageChangeNotification</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t>You have changed the contribution language from {{fromLanguage}} to {{toLanguage}}, we will be redirecting you to homepage to start participating again.</t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr"/>
+      <c r="D388" t="inlineStr"/>
+      <c r="E388" t="inlineStr"/>
+      <c r="F388" t="inlineStr"/>
+      <c r="G388" t="inlineStr"/>
+      <c r="H388" t="inlineStr"/>
+      <c r="I388" t="inlineStr"/>
+      <c r="J388" t="inlineStr"/>
+      <c r="K388" t="inlineStr"/>
+      <c r="L388" t="inlineStr"/>
+      <c r="M388" t="inlineStr"/>
+      <c r="N388" t="inlineStr"/>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>proceed</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Proceed</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>आगे बढ़ें</t>
+        </is>
+      </c>
+      <c r="D389" t="inlineStr"/>
+      <c r="E389" t="inlineStr">
+        <is>
+          <t>આગળ વધો</t>
+        </is>
+      </c>
+      <c r="F389" t="inlineStr">
+        <is>
+          <t>আগুৱাওক</t>
+        </is>
+      </c>
+      <c r="G389" t="inlineStr">
+        <is>
+          <t>শুরু করুন</t>
+        </is>
+      </c>
+      <c r="H389" t="inlineStr">
+        <is>
+          <t>தொடர்ந்து செயல்படு</t>
+        </is>
+      </c>
+      <c r="I389" t="inlineStr">
+        <is>
+          <t>ముందుకు సాగు</t>
+        </is>
+      </c>
+      <c r="J389" t="inlineStr">
+        <is>
+          <t>पुढे चला</t>
+        </is>
+      </c>
+      <c r="K389" t="inlineStr">
+        <is>
+          <t>ਅੱਗੇ ਵਧੋ</t>
+        </is>
+      </c>
+      <c r="L389" t="inlineStr">
+        <is>
+          <t>മുന്നോട്ട് പോകുക</t>
+        </is>
+      </c>
+      <c r="M389" t="inlineStr">
+        <is>
+          <t>ଆଗକୁ ବଢ଼ନ୍ତୁ</t>
+        </is>
+      </c>
+      <c r="N389" t="inlineStr">
+        <is>
+          <t>ಮುಂದುವರಿಯಿರಿ</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>apiFailureError</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>An unexpected error has occurred.</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>एक अनपेक्षित गलती हुई है।</t>
+        </is>
+      </c>
+      <c r="D390" t="inlineStr"/>
+      <c r="E390" t="inlineStr">
+        <is>
+          <t>એક અનપેક્ષિત ભૂલ આવી છે.</t>
+        </is>
+      </c>
+      <c r="F390" t="inlineStr">
+        <is>
+          <t>এটা অবাঞ্চিত ত্ৰুটি সংঘটিত হৈছে৷</t>
+        </is>
+      </c>
+      <c r="G390" t="inlineStr">
+        <is>
+          <t>একটি অপ্রত্যাশিত ত্রুটি ঘটেছে</t>
+        </is>
+      </c>
+      <c r="H390" t="inlineStr">
+        <is>
+          <t>எதிர்பாராத பிழை ஏற்பட்டது.</t>
+        </is>
+      </c>
+      <c r="I390" t="inlineStr">
+        <is>
+          <t>అనుకోకుండా ఊహించని ఎర్రర్ సంభవించింది.</t>
+        </is>
+      </c>
+      <c r="J390" t="inlineStr">
+        <is>
+          <t>अनपेक्षित चूक झाली आहे.</t>
+        </is>
+      </c>
+      <c r="K390" t="inlineStr">
+        <is>
+          <t>ਇੱਕ ਅਣ-ਕਿਆਸੀ ਗਲਤੀ ਹੋਈ ਹੈ।</t>
+        </is>
+      </c>
+      <c r="L390" t="inlineStr">
+        <is>
+          <t>അപ്രതീക്ഷിതമായ ഒരു പിശക് സംഭവിച്ചിരിക്കുന്നു.</t>
+        </is>
+      </c>
+      <c r="M390" t="inlineStr">
+        <is>
+          <t>ଏକ ଆକସ୍ମିକ ତ୍ରୁଟି ଘଟିଛି ।</t>
+        </is>
+      </c>
+      <c r="N390" t="inlineStr">
+        <is>
+          <t>ಒಂದು ಅನಿರೀಕ್ಷಿತ ದೋಷ ಸಂಭವಿಸಿದೆ.</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>multipleRequestApiError</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>We are processing multiple requests at the moment. Please try again after sometime.</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>हम इस समय कई अनुरोधों को प्रॉसेस कर रहे हैं। कृपया कुछ समय बाद पुन: प्रयास करें।</t>
+        </is>
+      </c>
+      <c r="D391" t="inlineStr"/>
+      <c r="E391" t="inlineStr">
+        <is>
+          <t>અમે હાલમાં ઘણી વિનંતીઓ પર પ્રક્રિયા કરી રહ્યા છીએ. કૃપા કરીને થોડો સમય પછી ફરી પ્રયાસ કરો.</t>
+        </is>
+      </c>
+      <c r="F391" t="inlineStr">
+        <is>
+          <t>আমি এই সময়ত একাধিক অনুৰোধৰ ওপৰত কাৰ্য কৰি আছো৷ অনুগ্ৰহ কৰি কিছু সময় পিছত পুনৰ চেষ্টা কৰক৷</t>
+        </is>
+      </c>
+      <c r="G391" t="inlineStr">
+        <is>
+          <t>আমরা এই মুহূর্তে একাধিক অনুরোধ নিয়ে কাজ করছি। অনুগ্রহ করে কিছুক্ষণ পর আবার চেষ্টা করুন।</t>
+        </is>
+      </c>
+      <c r="H391" t="inlineStr">
+        <is>
+          <t>இந்த தருணத்தில் பல கோரிக்கைகளை நாங்கள் செயலாக்குகிறோம். சிறிது நேரம் கழித்து மீண்டும் முயற்சிக்கவும்.</t>
+        </is>
+      </c>
+      <c r="I391" t="inlineStr">
+        <is>
+          <t>మేము ప్రస్తుతం చాలా అభ్యర్థనలను ప్రాసెస్ చేస్తున్నాము. దయచేసి కొంతసమయం తర్వాత మళ్లీ ప్రయత్నించండి.</t>
+        </is>
+      </c>
+      <c r="J391" t="inlineStr">
+        <is>
+          <t>आम्ही याक्षणी एकाधिक विनंत्यांवर प्रक्रिया करत आहोत. कृपया थोड्या वेळाने पुन्हा प्रयत्न करा.</t>
+        </is>
+      </c>
+      <c r="K391" t="inlineStr">
+        <is>
+          <t>ਅਸੀਂ ਇਸ ਸਮੇਂ ਕਈ ਰਿਕੁਐਸਟਾਂ ਨੂੰ ਪ੍ਰੋਸੈੱਸ ਕਰ ਰਹੇ ਹਾਂ। ਕਿਰਪਾ ਕਰਕੇ ਕੁਝ ਦੇਰ ਬਾਅਦ ਦੁਬਾਰਾ ਕੋਸ਼ਿਸ਼ ਕਰੋ।</t>
+        </is>
+      </c>
+      <c r="L391" t="inlineStr">
+        <is>
+          <t>ഇപ്പോള്‍ ഞങ്ങള്‍ ഒന്നിലധികം അപേക്ഷകള്‍ കൈകാര്യം ചെയ്യുന്നു. ദയവായി അല്പം സമയത്തിന് ശേഷം വീണ്ടും ശ്രമിക്കുക.</t>
+        </is>
+      </c>
+      <c r="M391" t="inlineStr">
+        <is>
+          <t>ଆମେ ବର୍ତ୍ତମାନ ଅନେକ ଅନୁରୋଧକୁ ପ୍ରୋସେସ କରୁଛୁ । ଦୟାକରି କିଛି ସମୟ ପରେ ଆଉଥରେ ଚେଷ୍ଟା କରନ୍ତୁ ।</t>
+        </is>
+      </c>
+      <c r="N391" t="inlineStr">
+        <is>
+          <t>ನಾವು ಈ ಸಮಯದಲ್ಲಿ ಅನೇಕ ವಿನಂತಿಗಳನ್ನು ಪ್ರಕ್ರಿಯೆಗೊಳಿಸುತ್ತಿದ್ದೇವೆ. ದಯವಿಟ್ಟು ಸ್ವಲ್ಪ ಸಮಯದ ನಂತರ ಮತ್ತೆ ಪ್ರಯತ್ನಿಸಿ.</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>close</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Close</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>बंद करें</t>
+        </is>
+      </c>
+      <c r="D392" t="inlineStr"/>
+      <c r="E392" t="inlineStr">
+        <is>
+          <t>બંધ કરો</t>
+        </is>
+      </c>
+      <c r="F392" t="inlineStr">
+        <is>
+          <t>বন্ধ কৰক</t>
+        </is>
+      </c>
+      <c r="G392" t="inlineStr">
+        <is>
+          <t>সমাপ্ত</t>
+        </is>
+      </c>
+      <c r="H392" t="inlineStr">
+        <is>
+          <t>மூடு</t>
+        </is>
+      </c>
+      <c r="I392" t="inlineStr">
+        <is>
+          <t>మూసివేయండి</t>
+        </is>
+      </c>
+      <c r="J392" t="inlineStr">
+        <is>
+          <t>बंद करा</t>
+        </is>
+      </c>
+      <c r="K392" t="inlineStr">
+        <is>
+          <t>ਬੰਦ ਕਰੋੋ</t>
+        </is>
+      </c>
+      <c r="L392" t="inlineStr">
+        <is>
+          <t>അവസാനിപ്പിക്കുക</t>
+        </is>
+      </c>
+      <c r="M392" t="inlineStr">
+        <is>
+          <t>ସମାପ୍ତ</t>
+        </is>
+      </c>
+      <c r="N392" t="inlineStr">
+        <is>
+          <t>ಕ್ಲೋಸ್ ಮಾಡಿ</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>validationWarningText</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t>We feel the text you entered doesn't match the original text, are you sure about your edit?</t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr"/>
+      <c r="D393" t="inlineStr"/>
+      <c r="E393" t="inlineStr"/>
+      <c r="F393" t="inlineStr"/>
+      <c r="G393" t="inlineStr"/>
+      <c r="H393" t="inlineStr"/>
+      <c r="I393" t="inlineStr"/>
+      <c r="J393" t="inlineStr"/>
+      <c r="K393" t="inlineStr"/>
+      <c r="L393" t="inlineStr"/>
+      <c r="M393" t="inlineStr"/>
+      <c r="N393" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
feat(translation): load pending translations
</commit_message>
<xml_diff>
--- a/utils/localization/resources/backup/nextjs_meta.xlsx
+++ b/utils/localization/resources/backup/nextjs_meta.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:N393"/>
+  <dimension ref="A2:N406"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -25396,18 +25396,46 @@
           <t>Seems this page doesn't exist</t>
         </is>
       </c>
-      <c r="C377" t="inlineStr"/>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>ऐसा लगता है कि यह पेज मौजूद नहीं है</t>
+        </is>
+      </c>
       <c r="D377" t="inlineStr"/>
-      <c r="E377" t="inlineStr"/>
+      <c r="E377" t="inlineStr">
+        <is>
+          <t>એવું લાગે છે કે આ પેજ અસ્તિત્વમાં નથી</t>
+        </is>
+      </c>
       <c r="F377" t="inlineStr"/>
-      <c r="G377" t="inlineStr"/>
+      <c r="G377" t="inlineStr">
+        <is>
+          <t>মনে হচ্ছে এই পৃষ্ঠাটির অস্তিত্ব নেই</t>
+        </is>
+      </c>
       <c r="H377" t="inlineStr"/>
-      <c r="I377" t="inlineStr"/>
-      <c r="J377" t="inlineStr"/>
+      <c r="I377" t="inlineStr">
+        <is>
+          <t>ఈ పేజీ అందుబాటులో లేదు</t>
+        </is>
+      </c>
+      <c r="J377" t="inlineStr">
+        <is>
+          <t>असे दिसते की हे पृष्ठ अस्तित्वात नाही</t>
+        </is>
+      </c>
       <c r="K377" t="inlineStr"/>
       <c r="L377" t="inlineStr"/>
-      <c r="M377" t="inlineStr"/>
-      <c r="N377" t="inlineStr"/>
+      <c r="M377" t="inlineStr">
+        <is>
+          <t>ଏହି ପେଜଟି ନଥିଲା ଭଳି ଲାଗୁଛି</t>
+        </is>
+      </c>
+      <c r="N377" t="inlineStr">
+        <is>
+          <t>ಈ ಪುಟವು ಅಸ್ತಿತ್ವದಲ್ಲಿಲ್ಲ</t>
+        </is>
+      </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
@@ -26097,7 +26125,7 @@
       </c>
       <c r="B388" t="inlineStr">
         <is>
-          <t>You have changed the contribution language from {{fromLanguage}} to {{toLanguage}}, we will be redirecting you to homepage to start participating again.</t>
+          <t>You have changed the contribution language from &lt;old language&gt; to &lt;new language&gt;, we will be redirecting you to homepage to start participating again.</t>
         </is>
       </c>
       <c r="C388" t="inlineStr"/>
@@ -26396,18 +26424,930 @@
           <t>We feel the text you entered doesn't match the original text, are you sure about your edit?</t>
         </is>
       </c>
-      <c r="C393" t="inlineStr"/>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>हमें लगता है कि आपके द्वारा एन्टर किया गया टेक्स्ट मूल टेक से मेल नहीं खा रहा, क्या आप अपने संपादन के बारे में निश्चित हैं?</t>
+        </is>
+      </c>
       <c r="D393" t="inlineStr"/>
-      <c r="E393" t="inlineStr"/>
+      <c r="E393" t="inlineStr">
+        <is>
+          <t>અમને લાગે છે કે તમે દાખલ કરેલ ટેક્સ્ટ મૂળ ટેક્સ્ટ સાથે મેળ ખાતી નથી, શું તમે તમારા સંપાદન વિશે ચોક્કસ છો?</t>
+        </is>
+      </c>
       <c r="F393" t="inlineStr"/>
-      <c r="G393" t="inlineStr"/>
+      <c r="G393" t="inlineStr">
+        <is>
+          <t>আমরা মনে করি আপনার লেখা টেক্সট টি মূল টেক্সট এর  সাথে মিলছে না, আপনি কি আপনার সম্পাদনা সম্পর্কে নিশ্চিত ?</t>
+        </is>
+      </c>
       <c r="H393" t="inlineStr"/>
-      <c r="I393" t="inlineStr"/>
-      <c r="J393" t="inlineStr"/>
+      <c r="I393" t="inlineStr">
+        <is>
+          <t>మీరు నమోదు చేసిన వచనం అసలు వచనంతో సరిపోలడం లేదని మేము భావిస్తున్నాము, మీరు మీ సవరణ గురించి ఖచ్చితంగా ఉన్నారా?</t>
+        </is>
+      </c>
+      <c r="J393" t="inlineStr">
+        <is>
+          <t>तुम्ही घातलेला मजकूर मूळ मजकुराशी जुळत नाही असे आम्हाला वाटते, तुम्हाला तुमच्या संपादनाबद्दल खात्री आहे का?</t>
+        </is>
+      </c>
       <c r="K393" t="inlineStr"/>
       <c r="L393" t="inlineStr"/>
-      <c r="M393" t="inlineStr"/>
-      <c r="N393" t="inlineStr"/>
+      <c r="M393" t="inlineStr">
+        <is>
+          <t>ଆପଣ ଲେଖିଥିବା ଟେକ୍ସଟ ପ୍ରକୃତ ଟେକ୍ସଟ ସହିତ ମେଳ ନ ଖାଇଲା ଭଳିଆଦିଶୁଛି, ଆପଣ ନିଜ ଏଡିଟ ସହିତ ସନ୍ତୁଷ୍ଟ ଅଛନ୍ତି କି ?</t>
+        </is>
+      </c>
+      <c r="N393" t="inlineStr">
+        <is>
+          <t>ನೀವು ನಮೂದಿಸಿದ ಪಠ್ಯವು ಮೂಲ ಪಠ್ಯಕ್ಕೆ ಹೊಂದಿಕೆಯಾಗುವುದಿಲ್ಲ ಎಂದು ನಾವು ಭಾವಿಸುತ್ತೇವೆ, ನಿಮ್ಮ ಸಂಪಾದನೆಯ ಬಗ್ಗೆ ನೀವು ಖಚಿತರಾಗಿದ್ದೀರಿಯೇ?</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>testMic</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>Test mic</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>Test Mic</t>
+        </is>
+      </c>
+      <c r="D394" t="inlineStr"/>
+      <c r="E394" t="inlineStr">
+        <is>
+          <t>Test Mic</t>
+        </is>
+      </c>
+      <c r="F394" t="inlineStr">
+        <is>
+          <t>Test Mic</t>
+        </is>
+      </c>
+      <c r="G394" t="inlineStr">
+        <is>
+          <t>Test Mic</t>
+        </is>
+      </c>
+      <c r="H394" t="inlineStr">
+        <is>
+          <t>Test Mic</t>
+        </is>
+      </c>
+      <c r="I394" t="inlineStr">
+        <is>
+          <t>Test Mic</t>
+        </is>
+      </c>
+      <c r="J394" t="inlineStr">
+        <is>
+          <t>Test Mic</t>
+        </is>
+      </c>
+      <c r="K394" t="inlineStr">
+        <is>
+          <t>Test Mic</t>
+        </is>
+      </c>
+      <c r="L394" t="inlineStr">
+        <is>
+          <t>Test Mic</t>
+        </is>
+      </c>
+      <c r="M394" t="inlineStr">
+        <is>
+          <t>Test Mic</t>
+        </is>
+      </c>
+      <c r="N394" t="inlineStr">
+        <is>
+          <t>Test Mic</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>playingBackAudio</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>Playingback Audio</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>Playingback Audio</t>
+        </is>
+      </c>
+      <c r="D395" t="inlineStr"/>
+      <c r="E395" t="inlineStr">
+        <is>
+          <t>Playingback Audio</t>
+        </is>
+      </c>
+      <c r="F395" t="inlineStr">
+        <is>
+          <t>Playingback Audio</t>
+        </is>
+      </c>
+      <c r="G395" t="inlineStr">
+        <is>
+          <t>Playingback Audio</t>
+        </is>
+      </c>
+      <c r="H395" t="inlineStr">
+        <is>
+          <t>Playingback Audio</t>
+        </is>
+      </c>
+      <c r="I395" t="inlineStr">
+        <is>
+          <t>Playingback Audio</t>
+        </is>
+      </c>
+      <c r="J395" t="inlineStr">
+        <is>
+          <t>Playingback Audio</t>
+        </is>
+      </c>
+      <c r="K395" t="inlineStr">
+        <is>
+          <t>Playingback Audio</t>
+        </is>
+      </c>
+      <c r="L395" t="inlineStr">
+        <is>
+          <t>Playingback Audio</t>
+        </is>
+      </c>
+      <c r="M395" t="inlineStr">
+        <is>
+          <t>Playingback Audio</t>
+        </is>
+      </c>
+      <c r="N395" t="inlineStr">
+        <is>
+          <t>Playingback Audio</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>speakClearly</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>Please speak clearly</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>Please speak clearly</t>
+        </is>
+      </c>
+      <c r="D396" t="inlineStr"/>
+      <c r="E396" t="inlineStr">
+        <is>
+          <t>Please speak clearly</t>
+        </is>
+      </c>
+      <c r="F396" t="inlineStr">
+        <is>
+          <t>Please speak clearly</t>
+        </is>
+      </c>
+      <c r="G396" t="inlineStr">
+        <is>
+          <t>Please speak clearly</t>
+        </is>
+      </c>
+      <c r="H396" t="inlineStr">
+        <is>
+          <t>Please speak clearly</t>
+        </is>
+      </c>
+      <c r="I396" t="inlineStr">
+        <is>
+          <t>Please speak clearly</t>
+        </is>
+      </c>
+      <c r="J396" t="inlineStr">
+        <is>
+          <t>Please speak clearly</t>
+        </is>
+      </c>
+      <c r="K396" t="inlineStr">
+        <is>
+          <t>Please speak clearly</t>
+        </is>
+      </c>
+      <c r="L396" t="inlineStr">
+        <is>
+          <t>Please speak clearly</t>
+        </is>
+      </c>
+      <c r="M396" t="inlineStr">
+        <is>
+          <t>Please speak clearly</t>
+        </is>
+      </c>
+      <c r="N396" t="inlineStr">
+        <is>
+          <t>Please speak clearly</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>recordingCountValidationMsg</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>Recording for {{remainingSec}} seconds</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>Recording for {{remainingSec}} seconds</t>
+        </is>
+      </c>
+      <c r="D397" t="inlineStr"/>
+      <c r="E397" t="inlineStr">
+        <is>
+          <t>Recording for {{remainingSec}} seconds</t>
+        </is>
+      </c>
+      <c r="F397" t="inlineStr">
+        <is>
+          <t>Recording for {{remainingSec}} seconds</t>
+        </is>
+      </c>
+      <c r="G397" t="inlineStr">
+        <is>
+          <t>Recording for {{remainingSec}} seconds</t>
+        </is>
+      </c>
+      <c r="H397" t="inlineStr">
+        <is>
+          <t>Recording for {{remainingSec}} seconds</t>
+        </is>
+      </c>
+      <c r="I397" t="inlineStr">
+        <is>
+          <t>Recording for {{remainingSec}} seconds</t>
+        </is>
+      </c>
+      <c r="J397" t="inlineStr">
+        <is>
+          <t>Recording for {{remainingSec}} seconds</t>
+        </is>
+      </c>
+      <c r="K397" t="inlineStr">
+        <is>
+          <t>Recording for {{remainingSec}} seconds</t>
+        </is>
+      </c>
+      <c r="L397" t="inlineStr">
+        <is>
+          <t>Recording for {{remainingSec}} seconds</t>
+        </is>
+      </c>
+      <c r="M397" t="inlineStr">
+        <is>
+          <t>Recording for {{remainingSec}} seconds</t>
+        </is>
+      </c>
+      <c r="N397" t="inlineStr">
+        <is>
+          <t>Recording for {{remainingSec}} seconds</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>backgroundNoise</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>Background Noise Detected</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>Background Noise Detected</t>
+        </is>
+      </c>
+      <c r="D398" t="inlineStr"/>
+      <c r="E398" t="inlineStr">
+        <is>
+          <t>Background Noise Detected</t>
+        </is>
+      </c>
+      <c r="F398" t="inlineStr">
+        <is>
+          <t>Background Noise Detected</t>
+        </is>
+      </c>
+      <c r="G398" t="inlineStr">
+        <is>
+          <t>Background Noise Detected</t>
+        </is>
+      </c>
+      <c r="H398" t="inlineStr">
+        <is>
+          <t>Background Noise Detected</t>
+        </is>
+      </c>
+      <c r="I398" t="inlineStr">
+        <is>
+          <t>Background Noise Detected</t>
+        </is>
+      </c>
+      <c r="J398" t="inlineStr">
+        <is>
+          <t>Background Noise Detected</t>
+        </is>
+      </c>
+      <c r="K398" t="inlineStr">
+        <is>
+          <t>Background Noise Detected</t>
+        </is>
+      </c>
+      <c r="L398" t="inlineStr">
+        <is>
+          <t>Background Noise Detected</t>
+        </is>
+      </c>
+      <c r="M398" t="inlineStr">
+        <is>
+          <t>Background Noise Detected</t>
+        </is>
+      </c>
+      <c r="N398" t="inlineStr">
+        <is>
+          <t>Background Noise Detected</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>lowBackgroundNoise</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t>Low/No Background Noise</t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>Low/No Background Noise</t>
+        </is>
+      </c>
+      <c r="D399" t="inlineStr"/>
+      <c r="E399" t="inlineStr">
+        <is>
+          <t>Low/No Background Noise</t>
+        </is>
+      </c>
+      <c r="F399" t="inlineStr">
+        <is>
+          <t>Low/No Background Noise</t>
+        </is>
+      </c>
+      <c r="G399" t="inlineStr">
+        <is>
+          <t>Low/No Background Noise</t>
+        </is>
+      </c>
+      <c r="H399" t="inlineStr">
+        <is>
+          <t>Low/No Background Noise</t>
+        </is>
+      </c>
+      <c r="I399" t="inlineStr">
+        <is>
+          <t>Low/No Background Noise</t>
+        </is>
+      </c>
+      <c r="J399" t="inlineStr">
+        <is>
+          <t>Low/No Background Noise</t>
+        </is>
+      </c>
+      <c r="K399" t="inlineStr">
+        <is>
+          <t>Low/No Background Noise</t>
+        </is>
+      </c>
+      <c r="L399" t="inlineStr">
+        <is>
+          <t>Low/No Background Noise</t>
+        </is>
+      </c>
+      <c r="M399" t="inlineStr">
+        <is>
+          <t>Low/No Background Noise</t>
+        </is>
+      </c>
+      <c r="N399" t="inlineStr">
+        <is>
+          <t>Low/No Background Noise</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>quickTips</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>Quick Tips</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>Quick Tips</t>
+        </is>
+      </c>
+      <c r="D400" t="inlineStr"/>
+      <c r="E400" t="inlineStr">
+        <is>
+          <t>Quick Tips</t>
+        </is>
+      </c>
+      <c r="F400" t="inlineStr">
+        <is>
+          <t>Quick Tips</t>
+        </is>
+      </c>
+      <c r="G400" t="inlineStr">
+        <is>
+          <t>Quick Tips</t>
+        </is>
+      </c>
+      <c r="H400" t="inlineStr">
+        <is>
+          <t>Quick Tips</t>
+        </is>
+      </c>
+      <c r="I400" t="inlineStr">
+        <is>
+          <t>Quick Tips</t>
+        </is>
+      </c>
+      <c r="J400" t="inlineStr">
+        <is>
+          <t>Quick Tips</t>
+        </is>
+      </c>
+      <c r="K400" t="inlineStr">
+        <is>
+          <t>Quick Tips</t>
+        </is>
+      </c>
+      <c r="L400" t="inlineStr">
+        <is>
+          <t>Quick Tips</t>
+        </is>
+      </c>
+      <c r="M400" t="inlineStr">
+        <is>
+          <t>Quick Tips</t>
+        </is>
+      </c>
+      <c r="N400" t="inlineStr">
+        <is>
+          <t>Quick Tips</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>tipOne</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Microphone&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Microphone&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="D401" t="inlineStr"/>
+      <c r="E401" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Microphone&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="F401" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Microphone&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="G401" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Microphone&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="H401" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Microphone&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="I401" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Microphone&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="J401" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Microphone&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="K401" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Microphone&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="L401" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Microphone&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="M401" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Microphone&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="N401" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Microphone&lt;/b&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>tipTwo</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Speakers&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Speakers&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="D402" t="inlineStr"/>
+      <c r="E402" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Speakers&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="F402" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Speakers&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="G402" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Speakers&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="H402" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Speakers&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="I402" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Speakers&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="J402" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Speakers&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="K402" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Speakers&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="L402" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Speakers&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="M402" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Speakers&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="N402" t="inlineStr">
+        <is>
+          <t>Please test your &lt;b&gt;Speakers&lt;/b&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>tipThree</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>Ensure there is &lt;b&gt;no background noise&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>Ensure there is &lt;b&gt;no background noise&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="D403" t="inlineStr"/>
+      <c r="E403" t="inlineStr">
+        <is>
+          <t>Ensure there is &lt;b&gt;no background noise&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="F403" t="inlineStr">
+        <is>
+          <t>Ensure there is &lt;b&gt;no background noise&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="G403" t="inlineStr">
+        <is>
+          <t>Ensure there is &lt;b&gt;no background noise&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="H403" t="inlineStr">
+        <is>
+          <t>Ensure there is &lt;b&gt;no background noise&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="I403" t="inlineStr">
+        <is>
+          <t>Ensure there is &lt;b&gt;no background noise&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="J403" t="inlineStr">
+        <is>
+          <t>Ensure there is &lt;b&gt;no background noise&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="K403" t="inlineStr">
+        <is>
+          <t>Ensure there is &lt;b&gt;no background noise&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="L403" t="inlineStr">
+        <is>
+          <t>Ensure there is &lt;b&gt;no background noise&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="M403" t="inlineStr">
+        <is>
+          <t>Ensure there is &lt;b&gt;no background noise&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="N403" t="inlineStr">
+        <is>
+          <t>Ensure there is &lt;b&gt;no background noise&lt;/b&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>tipFour</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Read once &lt;b&gt;before recording it&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>Read once &lt;b&gt;before recording it&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="D404" t="inlineStr"/>
+      <c r="E404" t="inlineStr">
+        <is>
+          <t>Read once &lt;b&gt;before recording it&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="F404" t="inlineStr">
+        <is>
+          <t>Read once &lt;b&gt;before recording it&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="G404" t="inlineStr">
+        <is>
+          <t>Read once &lt;b&gt;before recording it&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="H404" t="inlineStr">
+        <is>
+          <t>Read once &lt;b&gt;before recording it&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="I404" t="inlineStr">
+        <is>
+          <t>Read once &lt;b&gt;before recording it&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="J404" t="inlineStr">
+        <is>
+          <t>Read once &lt;b&gt;before recording it&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="K404" t="inlineStr">
+        <is>
+          <t>Read once &lt;b&gt;before recording it&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="L404" t="inlineStr">
+        <is>
+          <t>Read once &lt;b&gt;before recording it&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="M404" t="inlineStr">
+        <is>
+          <t>Read once &lt;b&gt;before recording it&lt;/b&gt;</t>
+        </is>
+      </c>
+      <c r="N404" t="inlineStr">
+        <is>
+          <t>Read once &lt;b&gt;before recording it&lt;/b&gt;</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>tipFive</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>Get started by clicking on &lt;b&gt;Record&lt;/b&gt; button</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>Get started by clicking on &lt;b&gt;Record&lt;/b&gt; button</t>
+        </is>
+      </c>
+      <c r="D405" t="inlineStr"/>
+      <c r="E405" t="inlineStr">
+        <is>
+          <t>Get started by clicking on &lt;b&gt;Record&lt;/b&gt; button</t>
+        </is>
+      </c>
+      <c r="F405" t="inlineStr">
+        <is>
+          <t>Get started by clicking on &lt;b&gt;Record&lt;/b&gt; button</t>
+        </is>
+      </c>
+      <c r="G405" t="inlineStr">
+        <is>
+          <t>Get started by clicking on &lt;b&gt;Record&lt;/b&gt; button</t>
+        </is>
+      </c>
+      <c r="H405" t="inlineStr">
+        <is>
+          <t>Get started by clicking on &lt;b&gt;Record&lt;/b&gt; button</t>
+        </is>
+      </c>
+      <c r="I405" t="inlineStr">
+        <is>
+          <t>Get started by clicking on &lt;b&gt;Record&lt;/b&gt; button</t>
+        </is>
+      </c>
+      <c r="J405" t="inlineStr">
+        <is>
+          <t>Get started by clicking on &lt;b&gt;Record&lt;/b&gt; button</t>
+        </is>
+      </c>
+      <c r="K405" t="inlineStr">
+        <is>
+          <t>Get started by clicking on &lt;b&gt;Record&lt;/b&gt; button</t>
+        </is>
+      </c>
+      <c r="L405" t="inlineStr">
+        <is>
+          <t>Get started by clicking on &lt;b&gt;Record&lt;/b&gt; button</t>
+        </is>
+      </c>
+      <c r="M405" t="inlineStr">
+        <is>
+          <t>Get started by clicking on &lt;b&gt;Record&lt;/b&gt; button</t>
+        </is>
+      </c>
+      <c r="N405" t="inlineStr">
+        <is>
+          <t>Get started by clicking on &lt;b&gt;Record&lt;/b&gt; button</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>warningAudioPermissionMsg</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Sorry !!! We could not get access to your audio input device. Make sure you have given microphone access permission</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>Sorry !!! We could not get access to your audio input device. Make sure you have given microphone access permission</t>
+        </is>
+      </c>
+      <c r="D406" t="inlineStr"/>
+      <c r="E406" t="inlineStr">
+        <is>
+          <t>Sorry !!! We could not get access to your audio input device. Make sure you have given microphone access permission</t>
+        </is>
+      </c>
+      <c r="F406" t="inlineStr">
+        <is>
+          <t>Sorry !!! We could not get access to your audio input device. Make sure you have given microphone access permission</t>
+        </is>
+      </c>
+      <c r="G406" t="inlineStr">
+        <is>
+          <t>Sorry !!! We could not get access to your audio input device. Make sure you have given microphone access permission</t>
+        </is>
+      </c>
+      <c r="H406" t="inlineStr">
+        <is>
+          <t>Sorry !!! We could not get access to your audio input device. Make sure you have given microphone access permission</t>
+        </is>
+      </c>
+      <c r="I406" t="inlineStr">
+        <is>
+          <t>Sorry !!! We could not get access to your audio input device. Make sure you have given microphone access permission</t>
+        </is>
+      </c>
+      <c r="J406" t="inlineStr">
+        <is>
+          <t>Sorry !!! We could not get access to your audio input device. Make sure you have given microphone access permission</t>
+        </is>
+      </c>
+      <c r="K406" t="inlineStr">
+        <is>
+          <t>Sorry !!! We could not get access to your audio input device. Make sure you have given microphone access permission</t>
+        </is>
+      </c>
+      <c r="L406" t="inlineStr">
+        <is>
+          <t>Sorry !!! We could not get access to your audio input device. Make sure you have given microphone access permission</t>
+        </is>
+      </c>
+      <c r="M406" t="inlineStr">
+        <is>
+          <t>Sorry !!! We could not get access to your audio input device. Make sure you have given microphone access permission</t>
+        </is>
+      </c>
+      <c r="N406" t="inlineStr">
+        <is>
+          <t>Sorry !!! We could not get access to your audio input device. Make sure you have given microphone access permission</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>